<commit_message>
Add instructions on Excel Solver usage
</commit_message>
<xml_diff>
--- a/datasets/comparisons/comparison_figure_data.xlsx
+++ b/datasets/comparisons/comparison_figure_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmsalamy/Documents/GitHub/james-flumenequi/datasets/comparisons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E773F8D-514D-0244-A93D-4254F36F675A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAEBD43-B9C1-A14B-97C1-A87CFF30A5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="2680" windowWidth="27640" windowHeight="15960" activeTab="6" xr2:uid="{9AB40497-95D2-9245-ADE1-82C821021C28}"/>
+    <workbookView xWindow="1140" yWindow="940" windowWidth="27640" windowHeight="15960" activeTab="3" xr2:uid="{9AB40497-95D2-9245-ADE1-82C821021C28}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT_Consist_TCP" sheetId="2" r:id="rId1"/>
@@ -34,6 +34,127 @@
     <definedName name="iter_burst_r50_proc" localSheetId="3">'ResNet Results for Graphing'!$H$27:$L$47</definedName>
     <definedName name="iter_webs_bert_proc" localSheetId="0">BERT_Consist_TCP!$F$3:$J$20</definedName>
     <definedName name="iter_webs_rn50_proc" localSheetId="1">ResNet_Consist_TCP!$F$3:$J$20</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'BERT Results for Graphing'!$V$55</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">BERT_Consist_TCP!$Q$3:$R$3</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'ResNet Results for Graphing'!$T$27:$U$27</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">ResNet_Consist_TCP!$P$3:$Q$3</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'BERT Results for Graphing'!$S$55</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">BERT_Consist_TCP!$N$3</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">ResNet_Consist_TCP!$N$3</definedName>
+    <definedName name="solver_lin" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'Additional Analysis'!$I$10</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'BERT Results for Graphing'!$V$56</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">BERT_Consist_TCP!$R$4</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'ResNet Results for Graphing'!$V$28</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">ResNet_Consist_TCP!$Q$4</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">0.1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">0.05</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">0.05</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
     <definedName name="tcp_burst_bert_proc" localSheetId="2">'BERT Results for Graphing'!$A$26:$E$44</definedName>
     <definedName name="tcp_burst_r50_proc" localSheetId="3">'ResNet Results for Graphing'!$A$27:$E$47</definedName>
     <definedName name="tcp_ref_consist" localSheetId="4">'Additional Analysis'!$A$12:$F$27</definedName>
@@ -171,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="101">
   <si>
     <t>reversed</t>
   </si>
@@ -435,6 +556,45 @@
   </si>
   <si>
     <t>RDMA Fit</t>
+  </si>
+  <si>
+    <t>Solver Instructions:</t>
+  </si>
+  <si>
+    <t>Enable:</t>
+  </si>
+  <si>
+    <t>Tools &gt; Excel Add-ins &gt; Solver</t>
+  </si>
+  <si>
+    <t>Solver…</t>
+  </si>
+  <si>
+    <t>To Start:</t>
+  </si>
+  <si>
+    <t>Setup:</t>
+  </si>
+  <si>
+    <t>set objective:</t>
+  </si>
+  <si>
+    <t>RMSE cell</t>
+  </si>
+  <si>
+    <t>to minimum</t>
+  </si>
+  <si>
+    <t>by changing variable cells</t>
+  </si>
+  <si>
+    <t>subject to constraints</t>
+  </si>
+  <si>
+    <t>add &gt; first value RMSE cannot be above a threshold, eg 0.1</t>
+  </si>
+  <si>
+    <t>this is to prevent the solver over optimizing for the high BW cases</t>
   </si>
 </sst>
 </file>
@@ -3112,85 +3272,85 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>1.8999556391241135</c:v>
+                  <c:v>1.1578380423170569</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9900384471964747</c:v>
+                  <c:v>1.2321933481678797</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0979204176700872</c:v>
+                  <c:v>1.3227716166041696</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2297053189323508</c:v>
+                  <c:v>1.4356054622129337</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3946793956458774</c:v>
+                  <c:v>1.5801100545366218</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6076951087736537</c:v>
+                  <c:v>1.7717976409904157</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7394885910340814</c:v>
+                  <c:v>1.893148688695341</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8940606044434345</c:v>
+                  <c:v>2.0380470862762325</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0779858223753651</c:v>
+                  <c:v>2.2139522623931112</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.3006253875659088</c:v>
+                  <c:v>2.4317553107640979</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5757607502483397</c:v>
+                  <c:v>2.7079502105487117</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.924513123359898</c:v>
+                  <c:v>3.0686431832365768</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.3808873865585509</c:v>
+                  <c:v>3.5574581799120657</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.0031211644183937</c:v>
+                  <c:v>4.2524442322324365</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.8992411887604863</c:v>
+                  <c:v>5.306178471528499</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.2922920699511531</c:v>
+                  <c:v>7.0548297833838856</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.3180742878937561</c:v>
+                  <c:v>8.4195023344071682</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.7182639749306965</c:v>
+                  <c:v>10.376947373809607</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.726246469384215</c:v>
+                  <c:v>13.355787529198917</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14.803119879287109</c:v>
+                  <c:v>18.265709913727225</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19.978226473463391</c:v>
+                  <c:v>27.326335837191724</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>29.987772333918453</c:v>
+                  <c:v>47.160636543456711</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>54.376635317450372</c:v>
+                  <c:v>104.92132295662176</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>147.56977294755592</c:v>
+                  <c:v>401.27239123622371</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>342.39430962585197</c:v>
+                  <c:v>1243.2920704084856</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1405.1038899233204</c:v>
+                  <c:v>8288.1836967509298</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13184.834077730731</c:v>
+                  <c:v>167862.78930883235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3821,94 +3981,94 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1.4357056290353638</c:v>
+                  <c:v>1.1751012324961805</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4802889582007031</c:v>
+                  <c:v>1.2123684084904003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5327888729033958</c:v>
+                  <c:v>1.2562831632413731</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5956922942443994</c:v>
+                  <c:v>1.3089415979426464</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6726845174698446</c:v>
+                  <c:v>1.3734532741021153</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7694821012573199</c:v>
+                  <c:v>1.4546478451475098</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8280243000627192</c:v>
+                  <c:v>1.503799017649982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8954788107139617</c:v>
+                  <c:v>1.5604736814844826</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9741681578440711</c:v>
+                  <c:v>1.6266410770431516</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0673144279585771</c:v>
+                  <c:v>1.7050361371141876</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.1795244814257573</c:v>
+                  <c:v>1.7995739803194892</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3176275525484127</c:v>
+                  <c:v>1.9160664750146688</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4922042652909706</c:v>
+                  <c:v>2.0635324852639303</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7205764853620327</c:v>
+                  <c:v>2.2567648933049442</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0331839789169321</c:v>
+                  <c:v>2.5218180044433987</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.2375366464656712</c:v>
+                  <c:v>2.6953979052429324</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.4888176496596852</c:v>
+                  <c:v>2.9091529913217933</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.8055038583831751</c:v>
+                  <c:v>3.1790031982843669</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.2171247445156759</c:v>
+                  <c:v>3.5304469111908574</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7738183451711347</c:v>
+                  <c:v>4.0068884074977431</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.5676284506363629</c:v>
+                  <c:v>4.6882539073805853</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.7861813787631675</c:v>
+                  <c:v>5.7380861479004821</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.8729744284778675</c:v>
+                  <c:v>7.5448441671323065</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13.143150071369075</c:v>
+                  <c:v>11.268215287726866</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17.388355132252759</c:v>
+                  <c:v>14.995493963292539</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.405915872580582</c:v>
+                  <c:v>22.084472190984645</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44.283552234764954</c:v>
+                  <c:v>38.944838065067749</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>112.47096458346022</c:v>
+                  <c:v>100.86214553920767</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>922.08651617806004</c:v>
+                  <c:v>864.17500813668278</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7457.2616260760087</c:v>
+                  <c:v>7301.7601683622834</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4020,7 +4180,6 @@
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
-          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4610,70 +4769,70 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0.85659488186816957</c:v>
+                  <c:v>0.85796747744169655</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9113185030920562</c:v>
+                  <c:v>0.91284100623760323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.97795939721747871</c:v>
+                  <c:v>0.97966933370008658</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0609422865512206</c:v>
+                  <c:v>1.0628925946877905</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1671694707523836</c:v>
+                  <c:v>1.1694378754947772</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3080065016455373</c:v>
+                  <c:v>1.3107129677901646</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3971254466858716</c:v>
+                  <c:v>1.400117886813798</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5034997121182974</c:v>
+                  <c:v>1.5068416879331217</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6325859411442676</c:v>
+                  <c:v>1.6363632000465422</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7923471947038476</c:v>
+                  <c:v>1.7966787059364735</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.9948364909629437</c:v>
+                  <c:v>1.9998929505941458</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.2591191041161394</c:v>
+                  <c:v>2.2651556271559667</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.6170304571965448</c:v>
+                  <c:v>2.624448134548178</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.1254800551394446</c:v>
+                  <c:v>3.1349514583053786</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8956062662854523</c:v>
+                  <c:v>3.9083588656012545</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.1719680377304753</c:v>
+                  <c:v>5.1905177803911755</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.5926554870463709</c:v>
+                  <c:v>7.6231079608503665</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.326684276109573</c:v>
+                  <c:v>13.388422612332803</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.896863128386755</c:v>
+                  <c:v>19.997859069180794</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.244242069471774</c:v>
+                  <c:v>34.438640054667047</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>75.878740909612404</c:v>
+                  <c:v>76.376345111619628</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>288.2420867248768</c:v>
+                  <c:v>290.55887491390115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5304,94 +5463,94 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1.4357056290353638</c:v>
+                  <c:v>1.1751012324961805</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4802889582007031</c:v>
+                  <c:v>1.2123684084904003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5327888729033958</c:v>
+                  <c:v>1.2562831632413731</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5956922942443994</c:v>
+                  <c:v>1.3089415979426464</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6726845174698446</c:v>
+                  <c:v>1.3734532741021153</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7694821012573199</c:v>
+                  <c:v>1.4546478451475098</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8280243000627192</c:v>
+                  <c:v>1.503799017649982</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8954788107139617</c:v>
+                  <c:v>1.5604736814844826</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9741681578440711</c:v>
+                  <c:v>1.6266410770431516</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0673144279585771</c:v>
+                  <c:v>1.7050361371141876</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.1795244814257573</c:v>
+                  <c:v>1.7995739803194892</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3176275525484127</c:v>
+                  <c:v>1.9160664750146688</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4922042652909706</c:v>
+                  <c:v>2.0635324852639303</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.7205764853620327</c:v>
+                  <c:v>2.2567648933049442</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0331839789169321</c:v>
+                  <c:v>2.5218180044433987</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.2375366464656712</c:v>
+                  <c:v>2.6953979052429324</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.4888176496596852</c:v>
+                  <c:v>2.9091529913217933</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.8055038583831751</c:v>
+                  <c:v>3.1790031982843669</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.2171247445156759</c:v>
+                  <c:v>3.5304469111908574</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7738183451711347</c:v>
+                  <c:v>4.0068884074977431</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.5676284506363629</c:v>
+                  <c:v>4.6882539073805853</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.7861813787631675</c:v>
+                  <c:v>5.7380861479004821</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.8729744284778675</c:v>
+                  <c:v>7.5448441671323065</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13.143150071369075</c:v>
+                  <c:v>11.268215287726866</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17.388355132252759</c:v>
+                  <c:v>14.995493963292539</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25.405915872580582</c:v>
+                  <c:v>22.084472190984645</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44.283552234764954</c:v>
+                  <c:v>38.944838065067749</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>112.47096458346022</c:v>
+                  <c:v>100.86214553920767</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>922.08651617806004</c:v>
+                  <c:v>864.17500813668278</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7457.2616260760087</c:v>
+                  <c:v>7301.7601683622834</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8104,85 +8263,85 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0.11742840097313823</c:v>
+                  <c:v>0.19866080851497578</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12232268228065703</c:v>
+                  <c:v>0.20584740049479477</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12814965065137718</c:v>
+                  <c:v>0.214355121253333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13521981292977017</c:v>
+                  <c:v>0.22461100160663416</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14400132282894418</c:v>
+                  <c:v>0.23725320053219492</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.14924964453554718</c:v>
+                  <c:v>0.24476086083799128</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15523511902118128</c:v>
+                  <c:v>0.25328136750761765</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16213063168105551</c:v>
+                  <c:v>0.2630447393908687</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17016811042738117</c:v>
+                  <c:v>0.27435737301277496</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1796660410712573</c:v>
+                  <c:v>0.28763673183316124</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19107386876364749</c:v>
+                  <c:v>0.30346681151082383</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20504666319571263</c:v>
+                  <c:v>0.32269045573721539</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.22257697515745176</c:v>
+                  <c:v>0.34657050100986875</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.24524187919723919</c:v>
+                  <c:v>0.3770877101157093</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.27570085635048086</c:v>
+                  <c:v>0.41753202867476052</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.31879635409633084</c:v>
+                  <c:v>0.47378587161692465</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.38430001965780758</c:v>
+                  <c:v>0.55745580346230017</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.49501014208860411</c:v>
+                  <c:v>0.69484964278191119</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.58414092731773515</c:v>
+                  <c:v>0.80253898113566569</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.71733080698263818</c:v>
+                  <c:v>0.95961181360154468</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.93431409083768935</c:v>
+                  <c:v>1.2077558102414399</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.3365239847154058</c:v>
+                  <c:v>1.6492695896613865</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2584692307802929</c:v>
+                  <c:v>2.6035810765574894</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.4452231282351118</c:v>
+                  <c:v>5.6000070250749356</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11.434744147696952</c:v>
+                  <c:v>10.680659411215686</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39.695474704878798</c:v>
+                  <c:v>31.549334095708467</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>285.67579059652263</c:v>
+                  <c:v>175.76181179179352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8810,91 +8969,91 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>0.13588653011870339</c:v>
+                  <c:v>0.12506383805717336</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1397785405378715</c:v>
+                  <c:v>0.12863997629863019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14435017327728983</c:v>
+                  <c:v>0.13284037332170934</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14981199664694117</c:v>
+                  <c:v>0.1378583913963978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15647478966307238</c:v>
+                  <c:v>0.14397939242895369</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16039691140034634</c:v>
+                  <c:v>0.14758238385111599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16481837015117251</c:v>
+                  <c:v>0.15164391165487714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1698474196364364</c:v>
+                  <c:v>0.15626335438326289</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17562682878722827</c:v>
+                  <c:v>0.1615717677428502</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.18234898477850239</c:v>
+                  <c:v>0.1677457424353315</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19027972799213316</c:v>
+                  <c:v>0.17502927216578978</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1997974473725167</c:v>
+                  <c:v>0.18376961934077646</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.21146020797737977</c:v>
+                  <c:v>0.194478890723878</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.22612754127255114</c:v>
+                  <c:v>0.20794574137043437</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.24519690536095079</c:v>
+                  <c:v>0.22545222141676927</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.27110376460678515</c:v>
+                  <c:v>0.2492322999278081</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.30850404018041594</c:v>
+                  <c:v>0.28355583681975932</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.36753098838243631</c:v>
+                  <c:v>0.33771345500723943</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.41211637081651037</c:v>
+                  <c:v>0.3786113309299482</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.4750164607107214</c:v>
+                  <c:v>0.4362971077296689</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.57027171395105114</c:v>
+                  <c:v>0.52363269218996122</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.73048092745670445</c:v>
+                  <c:v>0.67047005065577236</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.049960731199588</c:v>
+                  <c:v>0.96313678939772329</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.3596391829662815</c:v>
+                  <c:v>1.2466843409678667</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.9297003917338651</c:v>
+                  <c:v>1.7683818531098865</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.2234376849448614</c:v>
+                  <c:v>2.9515081702193009</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.6228912196858145</c:v>
+                  <c:v>6.9700852166200313</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>53.196337169397601</c:v>
+                  <c:v>48.487681795993666</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>116.38904900552225</c:v>
+                  <c:v>105.95226467469747</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9937,91 +10096,91 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>0.13588653011870339</c:v>
+                  <c:v>0.12506383805717336</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1397785405378715</c:v>
+                  <c:v>0.12863997629863019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14435017327728983</c:v>
+                  <c:v>0.13284037332170934</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14981199664694117</c:v>
+                  <c:v>0.1378583913963978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15647478966307238</c:v>
+                  <c:v>0.14397939242895369</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16039691140034634</c:v>
+                  <c:v>0.14758238385111599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16481837015117251</c:v>
+                  <c:v>0.15164391165487714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1698474196364364</c:v>
+                  <c:v>0.15626335438326289</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17562682878722827</c:v>
+                  <c:v>0.1615717677428502</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.18234898477850239</c:v>
+                  <c:v>0.1677457424353315</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19027972799213316</c:v>
+                  <c:v>0.17502927216578978</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1997974473725167</c:v>
+                  <c:v>0.18376961934077646</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.21146020797737977</c:v>
+                  <c:v>0.194478890723878</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.22612754127255114</c:v>
+                  <c:v>0.20794574137043437</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.24519690536095079</c:v>
+                  <c:v>0.22545222141676927</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.27110376460678515</c:v>
+                  <c:v>0.2492322999278081</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.30850404018041594</c:v>
+                  <c:v>0.28355583681975932</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.36753098838243631</c:v>
+                  <c:v>0.33771345500723943</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.41211637081651037</c:v>
+                  <c:v>0.3786113309299482</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.4750164607107214</c:v>
+                  <c:v>0.4362971077296689</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.57027171395105114</c:v>
+                  <c:v>0.52363269218996122</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.73048092745670445</c:v>
+                  <c:v>0.67047005065577236</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.049960731199588</c:v>
+                  <c:v>0.96313678939772329</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.3596391829662815</c:v>
+                  <c:v>1.2466843409678667</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.9297003917338651</c:v>
+                  <c:v>1.7683818531098865</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.2234376849448614</c:v>
+                  <c:v>2.9515081702193009</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.6228912196858145</c:v>
+                  <c:v>6.9700852166200313</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>53.196337169397601</c:v>
+                  <c:v>48.487681795993666</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>116.38904900552225</c:v>
+                  <c:v>105.95226467469747</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10148,79 +10307,79 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.14623865206421349</c:v>
+                  <c:v>0.14528980346200421</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14720999126222756</c:v>
+                  <c:v>0.14625453127156215</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14848152959128577</c:v>
+                  <c:v>0.14751741184844255</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15019249706430657</c:v>
+                  <c:v>0.14921672410761161</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15257444241745477</c:v>
+                  <c:v>0.15158243323310053</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.15603701015760224</c:v>
+                  <c:v>0.15502137784877004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16136536358835915</c:v>
+                  <c:v>0.16031333157292713</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17023666950675909</c:v>
+                  <c:v>0.16912391187647993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1771080308859605</c:v>
+                  <c:v>0.17594813647485316</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.18683789548827009</c:v>
+                  <c:v>0.18561111147189799</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.20134299376219839</c:v>
+                  <c:v>0.2000161961486889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22454272768279698</c:v>
+                  <c:v>0.22305528674002914</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24187108093313855</c:v>
+                  <c:v>0.24026315156303191</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26562704107905971</c:v>
+                  <c:v>0.26385329597369095</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.29960918198176956</c:v>
+                  <c:v>0.29759708498030712</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.35099075720791428</c:v>
+                  <c:v>0.34861598513540876</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.43471290135251767</c:v>
+                  <c:v>0.431742196575855</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.58625795582859697</c:v>
+                  <c:v>0.58219606553133818</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.90685664189406989</c:v>
+                  <c:v>0.90044812010764819</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.2208953622494321</c:v>
+                  <c:v>1.2121525770273505</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.7759543576695722</c:v>
+                  <c:v>1.7630259539968887</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.8745054568774306</c:v>
+                  <c:v>2.8531414477224541</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.4140888997139065</c:v>
+                  <c:v>5.3727644295247794</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12.739511620896922</c:v>
+                  <c:v>12.638822023231807</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42.140303536355496</c:v>
+                  <c:v>41.791280268171271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10453,7 +10612,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{19515239-B85B-B042-8F0B-789AA53652EF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10475,7 +10634,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{04B4328C-D184-F241-978E-09BCE654A207}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10541,7 +10700,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302193" cy="6060351"/>
+    <xdr:ext cx="9302750" cy="6064250"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10607,7 +10766,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6064250"/>
+    <xdr:ext cx="9302193" cy="6060351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11554,7 +11713,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_webs_bert_proc" connectionId="3" xr16:uid="{AC8D97B8-AC69-7243-9B80-913500AC2DCB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_webs_r50_proc_v2" connectionId="9" xr16:uid="{3655E2A1-647D-044C-83AA-E500C389747D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11562,35 +11721,35 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_webs_r50_proc_v2" connectionId="9" xr16:uid="{3655E2A1-647D-044C-83AA-E500C389747D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_webs_bert_proc" connectionId="8" xr16:uid="{D98AF061-EC03-6749-8E41-D27915908B2A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_webs_bert_proc" connectionId="8" xr16:uid="{D98AF061-EC03-6749-8E41-D27915908B2A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_webs_bert_proc" connectionId="3" xr16:uid="{AC8D97B8-AC69-7243-9B80-913500AC2DCB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_webs_rn50_proc" connectionId="4" xr16:uid="{85BC3454-4AFF-F241-A074-EE6EF7C976D0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_webs_rn50_proc" connectionId="10" xr16:uid="{C8C5B576-A1C2-AE48-AFE8-F172225D2102}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_webs_rn50_proc" connectionId="4" xr16:uid="{85BC3454-4AFF-F241-A074-EE6EF7C976D0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_bert_proc" connectionId="1" xr16:uid="{F84050B8-2978-684E-BC02-AEAD61BB4D12}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_bert_proc" connectionId="5" xr16:uid="{BC8D0C62-B916-8246-82B9-B811595CEC59}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_bert_proc" connectionId="1" xr16:uid="{F84050B8-2978-684E-BC02-AEAD61BB4D12}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_r50_proc" connectionId="6" xr16:uid="{6F787254-D219-6A40-9CE5-389F29C54FBE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_r50_proc" connectionId="2" xr16:uid="{E187BCE5-6075-E44E-A643-4DE9D8CC6F65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_r50_proc" connectionId="2" xr16:uid="{E187BCE5-6075-E44E-A643-4DE9D8CC6F65}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_r50_proc" connectionId="6" xr16:uid="{6F787254-D219-6A40-9CE5-389F29C54FBE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11892,8 +12051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04C65A2-538F-FF44-91AD-6064857BAA71}">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView topLeftCell="M1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12025,28 +12184,28 @@
       </c>
       <c r="M3" s="8">
         <f>$Q$3*EXP(SQRT($R$3/(25-B3)))</f>
-        <v>1.4807094064383208</v>
+        <v>1.2127199739638559</v>
       </c>
       <c r="N3" s="8">
         <f t="shared" ref="N3:N5" si="3">(M3-G3)^2</f>
-        <v>1.9698182704392421E-3</v>
+        <v>4.9999999973035295E-2</v>
       </c>
       <c r="Q3">
-        <v>0.7</v>
+        <v>0.56438094987957921</v>
       </c>
       <c r="R3">
-        <v>12.9</v>
+        <v>13.446159703912063</v>
       </c>
       <c r="S3" s="2">
         <f>SQRT(R3)</f>
-        <v>3.591656999213594</v>
+        <v>3.6669005582251697</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
       <c r="V3" s="8">
         <f>$Q$3*EXP(SQRT($R$3/(25-U3)))</f>
-        <v>1.4357056290353638</v>
+        <v>1.1751012324961805</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -12091,25 +12250,25 @@
       </c>
       <c r="M4" s="8">
         <f t="shared" ref="M4:M27" si="4">$Q$3*EXP(SQRT($R$3/(25-B4)))</f>
-        <v>1.532977331966082</v>
+        <v>1.2564408615603488</v>
       </c>
       <c r="N4" s="8">
         <f t="shared" si="3"/>
-        <v>8.5062381490215445E-6</v>
+        <v>7.8093988146282323E-2</v>
       </c>
       <c r="Q4" t="s">
         <v>74</v>
       </c>
       <c r="R4">
         <f>SQRT(AVERAGE(N3:N27))</f>
-        <v>24.889225826873062</v>
+        <v>12.751421519325422</v>
       </c>
       <c r="U4">
         <v>2</v>
       </c>
       <c r="V4" s="8">
         <f t="shared" ref="V4:V32" si="5">$Q$3*EXP(SQRT($R$3/(25-U4)))</f>
-        <v>1.4802889582007031</v>
+        <v>1.2123684084904003</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -12154,18 +12313,18 @@
       </c>
       <c r="M5" s="8">
         <f t="shared" si="4"/>
-        <v>1.596829447052877</v>
+        <v>1.3098939498782285</v>
       </c>
       <c r="N5" s="8">
         <f t="shared" si="3"/>
-        <v>1.9926143055149788E-2</v>
+        <v>2.1250498204575093E-2</v>
       </c>
       <c r="U5">
         <v>4</v>
       </c>
       <c r="V5" s="8">
         <f t="shared" si="5"/>
-        <v>1.5327888729033958</v>
+        <v>1.2562831632413731</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -12210,18 +12369,18 @@
       </c>
       <c r="M6" s="8">
         <f t="shared" si="4"/>
-        <v>1.6545937105966408</v>
+        <v>1.3582893120650017</v>
       </c>
       <c r="N6" s="8">
         <f>(M6-G6)^2</f>
-        <v>2.9063941393778442E-4</v>
+        <v>9.8189819588842209E-2</v>
       </c>
       <c r="U6">
         <v>6</v>
       </c>
       <c r="V6" s="8">
         <f t="shared" si="5"/>
-        <v>1.5956922942443994</v>
+        <v>1.3089415979426464</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -12266,18 +12425,18 @@
       </c>
       <c r="M7" s="8">
         <f t="shared" si="4"/>
-        <v>1.7506391607805545</v>
+        <v>1.4388347810029074</v>
       </c>
       <c r="N7" s="8">
         <f t="shared" ref="N7:N27" si="6">(M7-G7)^2</f>
-        <v>7.163324530331687E-2</v>
+        <v>1.9501499383009504E-3</v>
       </c>
       <c r="U7">
         <v>8</v>
       </c>
       <c r="V7" s="8">
         <f t="shared" si="5"/>
-        <v>1.6726845174698446</v>
+        <v>1.3734532741021153</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
@@ -12322,18 +12481,18 @@
       </c>
       <c r="M8" s="8">
         <f t="shared" si="4"/>
-        <v>1.8911250822445049</v>
+        <v>1.5568144264854187</v>
       </c>
       <c r="N8" s="8">
         <f t="shared" si="6"/>
-        <v>0.19474078020059163</v>
+        <v>1.1445529466409006E-2</v>
       </c>
       <c r="U8">
         <v>10</v>
       </c>
       <c r="V8" s="8">
         <f t="shared" si="5"/>
-        <v>1.7694821012573199</v>
+        <v>1.4546478451475098</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
@@ -12378,11 +12537,11 @@
       </c>
       <c r="M9" s="8">
         <f t="shared" si="4"/>
-        <v>2.0629002425002088</v>
+        <v>1.7013193115010383</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" si="6"/>
-        <v>0.22856788952894597</v>
+        <v>1.3573837126138485E-2</v>
       </c>
       <c r="Q9" t="s">
         <v>66</v>
@@ -12392,14 +12551,14 @@
       </c>
       <c r="S9" s="10">
         <f>SUM(N3:N28)</f>
-        <v>14247.891932004957</v>
+        <v>3577.17251679734</v>
       </c>
       <c r="U9">
         <v>11</v>
       </c>
       <c r="V9" s="8">
         <f t="shared" si="5"/>
-        <v>1.8280243000627192</v>
+        <v>1.503799017649982</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
@@ -12444,11 +12603,11 @@
       </c>
       <c r="M10" s="8">
         <f t="shared" si="4"/>
-        <v>2.1400993474699068</v>
+        <v>1.7663461011985653</v>
       </c>
       <c r="N10" s="8">
         <f t="shared" si="6"/>
-        <v>0.13382614668944937</v>
+        <v>6.2895756887798015E-5</v>
       </c>
       <c r="Q10" s="2">
         <f>AVERAGE(G3:G16,G19:G27)</f>
@@ -12460,7 +12619,7 @@
       </c>
       <c r="V10" s="8">
         <f t="shared" si="5"/>
-        <v>1.8954788107139617</v>
+        <v>1.5604736814844826</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -12505,11 +12664,11 @@
       </c>
       <c r="M11" s="8">
         <f t="shared" si="4"/>
-        <v>2.3192231723737202</v>
+        <v>1.9174132770354568</v>
       </c>
       <c r="N11" s="8">
         <f t="shared" si="6"/>
-        <v>0.12318216772608011</v>
+        <v>2.5843724017727003E-3</v>
       </c>
       <c r="R11" t="s">
         <v>68</v>
@@ -12523,7 +12682,7 @@
       </c>
       <c r="V11" s="8">
         <f t="shared" si="5"/>
-        <v>1.9741681578440711</v>
+        <v>1.6266410770431516</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -12568,25 +12727,25 @@
       </c>
       <c r="M12" s="8">
         <f t="shared" si="4"/>
-        <v>2.4448901603758193</v>
+        <v>2.0235439342510637</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" si="6"/>
-        <v>0.18901955026872069</v>
+        <v>1.8003093311733326E-4</v>
       </c>
       <c r="R12" t="s">
         <v>69</v>
       </c>
       <c r="S12" s="2">
         <f>1-S9/S11</f>
-        <v>0.82652362010017943</v>
+        <v>0.95644584185137005</v>
       </c>
       <c r="U12">
         <v>14</v>
       </c>
       <c r="V12" s="8">
         <f t="shared" si="5"/>
-        <v>2.0673144279585771</v>
+        <v>1.7050361371141876</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -12631,18 +12790,18 @@
       </c>
       <c r="M13" s="8">
         <f t="shared" si="4"/>
-        <v>2.3436911506434099</v>
+        <v>1.9380681904599855</v>
       </c>
       <c r="N13" s="8">
         <f t="shared" si="6"/>
-        <v>6.7169066873217767E-3</v>
+        <v>0.23773396079394601</v>
       </c>
       <c r="U13">
         <v>15</v>
       </c>
       <c r="V13" s="8">
         <f t="shared" si="5"/>
-        <v>2.1795244814257573</v>
+        <v>1.7995739803194892</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
@@ -12687,18 +12846,18 @@
       </c>
       <c r="M14" s="8">
         <f t="shared" si="4"/>
-        <v>2.4108034495162789</v>
+        <v>1.9947448326417014</v>
       </c>
       <c r="N14" s="8">
         <f t="shared" si="6"/>
-        <v>0.27413046830654991</v>
+        <v>0.88291077345857627</v>
       </c>
       <c r="U14">
         <v>16</v>
       </c>
       <c r="V14" s="8">
         <f t="shared" si="5"/>
-        <v>2.3176275525484127</v>
+        <v>1.9160664750146688</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
@@ -12743,11 +12902,11 @@
       </c>
       <c r="M15" s="8">
         <f t="shared" si="4"/>
-        <v>2.6603306656204073</v>
+        <v>2.2057549211586789</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" si="6"/>
-        <v>0.50277113942155893</v>
+        <v>1.3540564428709205</v>
       </c>
       <c r="Q15" t="s">
         <v>76</v>
@@ -12757,7 +12916,7 @@
       </c>
       <c r="V15" s="8">
         <f t="shared" si="5"/>
-        <v>2.4922042652909706</v>
+        <v>2.0635324852639303</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
@@ -12802,18 +12961,18 @@
       </c>
       <c r="M16" s="8">
         <f t="shared" si="4"/>
-        <v>2.6907330008819152</v>
+        <v>2.2314935050797868</v>
       </c>
       <c r="N16" s="8">
         <f t="shared" si="6"/>
-        <v>5.2332656408191278</v>
+        <v>7.5453095866228468</v>
       </c>
       <c r="U16">
         <v>18</v>
       </c>
       <c r="V16" s="8">
         <f t="shared" si="5"/>
-        <v>2.7205764853620327</v>
+        <v>2.2567648933049442</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
@@ -12860,7 +13019,7 @@
       </c>
       <c r="V17" s="8">
         <f t="shared" si="5"/>
-        <v>3.0331839789169321</v>
+        <v>2.5218180044433987</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -12907,7 +13066,7 @@
       </c>
       <c r="V18" s="8">
         <f t="shared" si="5"/>
-        <v>3.2375366464656712</v>
+        <v>2.6953979052429324</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -12952,18 +13111,18 @@
       </c>
       <c r="M19" s="8">
         <f t="shared" si="4"/>
-        <v>56.875535819107398</v>
+        <v>50.281683783488013</v>
       </c>
       <c r="N19" s="8">
         <f t="shared" si="6"/>
-        <v>2084.6562348588941</v>
+        <v>1526.0104546701277</v>
       </c>
       <c r="U19">
         <v>20</v>
       </c>
       <c r="V19" s="8">
         <f t="shared" si="5"/>
-        <v>3.4888176496596852</v>
+        <v>2.9091529913217933</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
@@ -13008,18 +13167,18 @@
       </c>
       <c r="M20" s="8">
         <f t="shared" si="4"/>
-        <v>31.897858774608189</v>
+        <v>27.860189931953773</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" si="6"/>
-        <v>945.0997419938609</v>
+        <v>1209.6583750205243</v>
       </c>
       <c r="U20">
         <v>20.5</v>
       </c>
       <c r="V20" s="8">
         <f t="shared" si="5"/>
-        <v>3.8055038583831751</v>
+        <v>3.1790031982843669</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
@@ -13062,18 +13221,18 @@
       </c>
       <c r="M21" s="8">
         <f t="shared" si="4"/>
-        <v>3.9474490699991871</v>
+        <v>3.3001108112698065</v>
       </c>
       <c r="N21" s="8">
         <f t="shared" si="6"/>
-        <v>16.75071628354797</v>
+        <v>22.468568408486053</v>
       </c>
       <c r="U21">
         <v>21</v>
       </c>
       <c r="V21" s="8">
         <f t="shared" si="5"/>
-        <v>4.2171247445156759</v>
+        <v>3.5304469111908574</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
@@ -13116,18 +13275,18 @@
       </c>
       <c r="M22" s="8">
         <f t="shared" si="4"/>
-        <v>8.5456266139081745</v>
+        <v>7.2607745105838131</v>
       </c>
       <c r="N22" s="8">
         <f t="shared" si="6"/>
-        <v>6.1084468597317221</v>
+        <v>14.110385712697216</v>
       </c>
       <c r="U22">
         <v>21.5</v>
       </c>
       <c r="V22" s="8">
         <f t="shared" si="5"/>
-        <v>4.7738183451711347</v>
+        <v>4.0068884074977431</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
@@ -13170,18 +13329,18 @@
       </c>
       <c r="M23" s="8">
         <f t="shared" si="4"/>
-        <v>24.019302173183622</v>
+        <v>20.85460269825759</v>
       </c>
       <c r="N23" s="8">
         <f t="shared" si="6"/>
-        <v>16.958647848922364</v>
+        <v>0.90894946517200526</v>
       </c>
       <c r="U23">
         <v>22</v>
       </c>
       <c r="V23" s="8">
         <f t="shared" si="5"/>
-        <v>5.5676284506363629</v>
+        <v>4.6882539073805853</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
@@ -13224,18 +13383,18 @@
       </c>
       <c r="M24" s="8">
         <f t="shared" si="4"/>
-        <v>18.08302423034899</v>
+        <v>15.607370656019379</v>
       </c>
       <c r="N24" s="8">
         <f t="shared" si="6"/>
-        <v>354.10523499970839</v>
+        <v>453.40622944011665</v>
       </c>
       <c r="U24">
         <v>22.5</v>
       </c>
       <c r="V24" s="8">
         <f t="shared" si="5"/>
-        <v>6.7861813787631675</v>
+        <v>5.7380861479004821</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
@@ -13278,18 +13437,18 @@
       </c>
       <c r="M25" s="8">
         <f t="shared" si="4"/>
-        <v>174.19714985573401</v>
+        <v>157.65554600447615</v>
       </c>
       <c r="N25" s="8">
         <f t="shared" si="6"/>
-        <v>864.35901151748237</v>
+        <v>165.33791919502332</v>
       </c>
       <c r="U25">
         <v>23</v>
       </c>
       <c r="V25" s="8">
         <f t="shared" si="5"/>
-        <v>8.8729744284778675</v>
+        <v>7.5448441671323065</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
@@ -13332,18 +13491,18 @@
       </c>
       <c r="M26" s="8">
         <f t="shared" si="4"/>
-        <v>216.92005525447888</v>
+        <v>197.22571511363634</v>
       </c>
       <c r="N26" s="8">
         <f t="shared" si="6"/>
-        <v>41.816336859228556</v>
+        <v>174.97429299991063</v>
       </c>
       <c r="U26">
         <v>23.5</v>
       </c>
       <c r="V26" s="8">
         <f t="shared" si="5"/>
-        <v>13.143150071369075</v>
+        <v>11.268215287726866</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
@@ -13386,18 +13545,18 @@
       </c>
       <c r="M27" s="8">
         <f t="shared" si="4"/>
-        <v>82.55837237585375</v>
-      </c>
-      <c r="N27" s="8">
-        <f t="shared" si="6"/>
-        <v>9911.057511741652</v>
+        <v>73.558999794480869</v>
+      </c>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="U27">
         <v>23.75</v>
       </c>
       <c r="V27" s="8">
         <f t="shared" si="5"/>
-        <v>17.388355132252759</v>
+        <v>14.995493963292539</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
@@ -13408,7 +13567,7 @@
       </c>
       <c r="V28" s="8">
         <f t="shared" si="5"/>
-        <v>25.405915872580582</v>
+        <v>22.084472190984645</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -13418,7 +13577,7 @@
       </c>
       <c r="V29" s="8">
         <f t="shared" si="5"/>
-        <v>44.283552234764954</v>
+        <v>38.944838065067749</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
@@ -13428,7 +13587,7 @@
       </c>
       <c r="V30" s="8">
         <f t="shared" si="5"/>
-        <v>112.47096458346022</v>
+        <v>100.86214553920767</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -13438,7 +13597,7 @@
       </c>
       <c r="V31" s="8">
         <f t="shared" si="5"/>
-        <v>922.08651617806004</v>
+        <v>864.17500813668278</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -13448,7 +13607,7 @@
       </c>
       <c r="V32" s="8">
         <f t="shared" si="5"/>
-        <v>7457.2616260760087</v>
+        <v>7301.7601683622834</v>
       </c>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.2">
@@ -13463,8 +13622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA490CF-14AF-EB42-A801-03520D6E80A7}">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AH16" sqref="AH16"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13590,29 +13749,29 @@
       </c>
       <c r="M3" s="8">
         <f>$P$3*EXP(SQRT($Q$3/(25-B3)))</f>
-        <v>0.13980770076085319</v>
+        <v>0.12866676928799115</v>
       </c>
       <c r="N3" s="8">
         <f>(M3-G3)^2</f>
-        <v>4.4099454913352386E-4</v>
+        <v>1.0330311332711413E-3</v>
       </c>
       <c r="O3" s="8"/>
       <c r="P3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.4494202704216338E-2</v>
       </c>
       <c r="Q3">
-        <v>11</v>
+        <v>10.96434252907202</v>
       </c>
       <c r="R3" s="2">
         <f>SQRT(Q3)</f>
-        <v>3.3166247903553998</v>
+        <v>3.3112448609355396</v>
       </c>
       <c r="T3">
         <v>0</v>
       </c>
       <c r="U3" s="8">
         <f>$P$3*EXP(SQRT($Q$3/(25-T3)))</f>
-        <v>0.13588653011870339</v>
+        <v>0.12506383805717336</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -13657,11 +13816,11 @@
       </c>
       <c r="M4" s="8">
         <f t="shared" ref="M4:M27" si="3">$P$3*EXP(SQRT($Q$3/(25-B4)))</f>
-        <v>0.144359283758975</v>
+        <v>0.1328487437763971</v>
       </c>
       <c r="N4" s="8">
         <f t="shared" ref="N4:N27" si="4">(M4-G4)^2</f>
-        <v>4.2040945521612001E-4</v>
+        <v>1.0249236491714077E-3</v>
       </c>
       <c r="O4" s="8"/>
       <c r="P4" t="s">
@@ -13669,14 +13828,14 @@
       </c>
       <c r="Q4" s="9">
         <f>SQRT(AVERAGE(N3:N27))</f>
-        <v>2.6387457236116574</v>
+        <v>0.55683575971151711</v>
       </c>
       <c r="T4">
         <v>2</v>
       </c>
       <c r="U4" s="8">
         <f t="shared" ref="U4:U31" si="5">$P$3*EXP(SQRT($Q$3/(25-T4)))</f>
-        <v>0.1397785405378715</v>
+        <v>0.12863997629863019</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -13721,11 +13880,11 @@
       </c>
       <c r="M5" s="8">
         <f t="shared" si="3"/>
-        <v>0.14993638987030361</v>
+        <v>0.13797267344014574</v>
       </c>
       <c r="N5" s="8">
         <f t="shared" si="4"/>
-        <v>5.3674540964508265E-4</v>
+        <v>1.234221100524552E-3</v>
       </c>
       <c r="O5" s="8"/>
       <c r="T5">
@@ -13733,7 +13892,7 @@
       </c>
       <c r="U5" s="8">
         <f t="shared" si="5"/>
-        <v>0.14435017327728983</v>
+        <v>0.13284037332170934</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -13778,11 +13937,11 @@
       </c>
       <c r="M6" s="8">
         <f t="shared" si="3"/>
-        <v>0.15532667686339929</v>
+        <v>0.14292467028449113</v>
       </c>
       <c r="N6" s="8">
         <f t="shared" si="4"/>
-        <v>8.2579935219041149E-5</v>
+        <v>4.6179245846401029E-4</v>
       </c>
       <c r="O6" s="8"/>
       <c r="T6">
@@ -13790,7 +13949,7 @@
       </c>
       <c r="U6" s="8">
         <f t="shared" si="5"/>
-        <v>0.14981199664694117</v>
+        <v>0.1378583913963978</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -13835,11 +13994,11 @@
       </c>
       <c r="M7" s="8">
         <f t="shared" si="3"/>
-        <v>0.16303276426336871</v>
+        <v>0.15000368540781781</v>
       </c>
       <c r="N7" s="8">
         <f t="shared" si="4"/>
-        <v>2.3224024237907988E-7</v>
+        <v>1.5743136832992275E-4</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" t="s">
@@ -13850,14 +14009,14 @@
       </c>
       <c r="R7" s="10">
         <f>SUM(N3:N27)</f>
-        <v>174.07447484697025</v>
+        <v>7.4415855190440583</v>
       </c>
       <c r="T7">
         <v>8</v>
       </c>
       <c r="U7" s="8">
         <f t="shared" si="5"/>
-        <v>0.15647478966307238</v>
+        <v>0.14397939242895369</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -13902,11 +14061,11 @@
       </c>
       <c r="M8" s="8">
         <f t="shared" si="3"/>
-        <v>0.1744250377923543</v>
+        <v>0.16046794094569308</v>
       </c>
       <c r="N8" s="8">
         <f t="shared" si="4"/>
-        <v>7.5220091900180577E-6</v>
+        <v>1.2576430806315755E-4</v>
       </c>
       <c r="O8" s="8"/>
       <c r="P8" s="2">
@@ -13919,7 +14078,7 @@
       </c>
       <c r="U8" s="8">
         <f t="shared" si="5"/>
-        <v>0.16039691140034634</v>
+        <v>0.14758238385111599</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -13964,11 +14123,11 @@
       </c>
       <c r="M9" s="8">
         <f t="shared" si="3"/>
-        <v>0.18811375092209967</v>
+        <v>0.1730401062951277</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" si="4"/>
-        <v>3.2369082827823479E-5</v>
+        <v>8.8064359838898576E-5</v>
       </c>
       <c r="O9" s="8"/>
       <c r="Q9" t="s">
@@ -13976,14 +14135,14 @@
       </c>
       <c r="R9" s="10">
         <f>SUM(L3:L27)</f>
-        <v>516.02235932678559</v>
+        <v>252.12063008687483</v>
       </c>
       <c r="T9">
         <v>10</v>
       </c>
       <c r="U9" s="8">
         <f t="shared" si="5"/>
-        <v>0.16481837015117251</v>
+        <v>0.15164391165487714</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -14028,11 +14187,11 @@
       </c>
       <c r="M10" s="8">
         <f t="shared" si="3"/>
-        <v>0.19604637424762736</v>
+        <v>0.18032500250060293</v>
       </c>
       <c r="N10" s="8">
         <f t="shared" si="4"/>
-        <v>5.1609326250696096E-4</v>
+        <v>4.8948414762426166E-5</v>
       </c>
       <c r="O10" s="8"/>
       <c r="Q10" t="s">
@@ -14040,14 +14199,14 @@
       </c>
       <c r="R10" s="2">
         <f>1-R7/R9</f>
-        <v>0.66266098415953967</v>
+        <v>0.97048402775893483</v>
       </c>
       <c r="T10">
         <v>11</v>
       </c>
       <c r="U10" s="8">
         <f t="shared" si="5"/>
-        <v>0.1698474196364364</v>
+        <v>0.15626335438326289</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -14092,11 +14251,11 @@
       </c>
       <c r="M11" s="8">
         <f t="shared" si="3"/>
-        <v>0.20866525089847943</v>
+        <v>0.19191252475519657</v>
       </c>
       <c r="N11" s="8">
         <f t="shared" si="4"/>
-        <v>1.0585413636094347E-3</v>
+        <v>2.4908751164417803E-4</v>
       </c>
       <c r="O11" s="8"/>
       <c r="T11">
@@ -14104,7 +14263,7 @@
       </c>
       <c r="U11" s="8">
         <f t="shared" si="5"/>
-        <v>0.17562682878722827</v>
+        <v>0.1615717677428502</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
@@ -14149,11 +14308,11 @@
       </c>
       <c r="M12" s="8">
         <f t="shared" si="3"/>
-        <v>0.2210313900238782</v>
+        <v>0.20326686217469192</v>
       </c>
       <c r="N12" s="8">
         <f t="shared" si="4"/>
-        <v>1.1165185428430211E-3</v>
+        <v>2.449168195042955E-4</v>
       </c>
       <c r="O12" s="8"/>
       <c r="T12">
@@ -14161,7 +14320,7 @@
       </c>
       <c r="U12" s="8">
         <f t="shared" si="5"/>
-        <v>0.18234898477850239</v>
+        <v>0.1677457424353315</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
@@ -14206,11 +14365,11 @@
       </c>
       <c r="M13" s="8">
         <f t="shared" si="3"/>
-        <v>0.21365520826280954</v>
+        <v>0.19649432994460636</v>
       </c>
       <c r="N13" s="8">
         <f t="shared" si="4"/>
-        <v>6.7463299605899959E-5</v>
+        <v>8.0053707989800481E-5</v>
       </c>
       <c r="O13" s="8"/>
       <c r="P13" t="s">
@@ -14221,7 +14380,7 @@
       </c>
       <c r="U13" s="8">
         <f t="shared" si="5"/>
-        <v>0.19027972799213316</v>
+        <v>0.17502927216578978</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
@@ -14266,11 +14425,11 @@
       </c>
       <c r="M14" s="8">
         <f t="shared" si="3"/>
-        <v>0.21929866397463316</v>
+        <v>0.20167597179412666</v>
       </c>
       <c r="N14" s="8">
         <f t="shared" si="4"/>
-        <v>2.0070106005674756E-3</v>
+        <v>3.8965515349188725E-3</v>
       </c>
       <c r="O14" s="8"/>
       <c r="T14">
@@ -14278,7 +14437,7 @@
       </c>
       <c r="U14" s="8">
         <f t="shared" si="5"/>
-        <v>0.1997974473725167</v>
+        <v>0.18376961934077646</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
@@ -14323,11 +14482,11 @@
       </c>
       <c r="M15" s="8">
         <f t="shared" si="3"/>
-        <v>0.24017864172706979</v>
+        <v>0.22084546530422403</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" si="4"/>
-        <v>6.5850976232716598E-3</v>
+        <v>1.0096590292206099E-2</v>
       </c>
       <c r="O15" s="8"/>
       <c r="T15">
@@ -14335,7 +14494,7 @@
       </c>
       <c r="U15" s="8">
         <f t="shared" si="5"/>
-        <v>0.21146020797737977</v>
+        <v>0.194478890723878</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
@@ -14380,11 +14539,11 @@
       </c>
       <c r="M16" s="8">
         <f t="shared" si="3"/>
-        <v>0.24271212418803137</v>
+        <v>0.22317121651636801</v>
       </c>
       <c r="N16" s="8">
         <f t="shared" si="4"/>
-        <v>2.1086850098818319E-2</v>
+        <v>2.7143889496393982E-2</v>
       </c>
       <c r="O16" s="8"/>
       <c r="T16">
@@ -14392,7 +14551,7 @@
       </c>
       <c r="U16" s="8">
         <f t="shared" si="5"/>
-        <v>0.22612754127255114</v>
+        <v>0.20794574137043437</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -14437,11 +14596,11 @@
       </c>
       <c r="M17" s="8">
         <f t="shared" si="3"/>
-        <v>0.29027167206354082</v>
+        <v>0.26682425464589316</v>
       </c>
       <c r="N17" s="8">
         <f t="shared" si="4"/>
-        <v>0.20134966458844172</v>
+        <v>0.22294209762774378</v>
       </c>
       <c r="O17" s="8"/>
       <c r="T17">
@@ -14449,7 +14608,7 @@
       </c>
       <c r="U17" s="8">
         <f t="shared" si="5"/>
-        <v>0.24519690536095079</v>
+        <v>0.22545222141676927</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
@@ -14494,11 +14653,11 @@
       </c>
       <c r="M18" s="8">
         <f t="shared" si="3"/>
-        <v>0.40183355899981665</v>
+        <v>0.36917964249325791</v>
       </c>
       <c r="N18" s="8">
         <f t="shared" si="4"/>
-        <v>1.0410484852812423</v>
+        <v>1.1087495103605376</v>
       </c>
       <c r="O18" s="8"/>
       <c r="T18">
@@ -14506,7 +14665,7 @@
       </c>
       <c r="U18" s="8">
         <f t="shared" si="5"/>
-        <v>0.27110376460678515</v>
+        <v>0.2492322999278081</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
@@ -14551,11 +14710,11 @@
       </c>
       <c r="M19" s="8">
         <f t="shared" si="3"/>
-        <v>4.0614386008180938</v>
+        <v>3.7174215056542046</v>
       </c>
       <c r="N19" s="8">
         <f t="shared" si="4"/>
-        <v>4.7257439293814683</v>
+        <v>3.3483895594145725</v>
       </c>
       <c r="O19" s="8"/>
       <c r="T19">
@@ -14563,7 +14722,7 @@
       </c>
       <c r="U19" s="8">
         <f t="shared" si="5"/>
-        <v>0.30850404018041594</v>
+        <v>0.28355583681975932</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
@@ -14608,11 +14767,11 @@
       </c>
       <c r="M20" s="8">
         <f t="shared" si="3"/>
-        <v>2.3809423397274103</v>
+        <v>2.1811574180192088</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" si="4"/>
-        <v>5.7055206488148495E-4</v>
+        <v>5.0028784867473981E-2</v>
       </c>
       <c r="O20" s="8"/>
       <c r="T20">
@@ -14620,7 +14779,7 @@
       </c>
       <c r="U20" s="8">
         <f t="shared" si="5"/>
-        <v>0.36753098838243631</v>
+        <v>0.33771345500723943</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
@@ -14665,11 +14824,11 @@
       </c>
       <c r="M21" s="8">
         <f t="shared" si="3"/>
-        <v>0.3457735386221561</v>
+        <v>0.317752623817393</v>
       </c>
       <c r="N21" s="8">
         <f t="shared" si="4"/>
-        <v>7.67851714872861E-2</v>
+        <v>9.3099611141531674E-2</v>
       </c>
       <c r="O21" s="8"/>
       <c r="T21">
@@ -14677,7 +14836,7 @@
       </c>
       <c r="U21" s="8">
         <f t="shared" si="5"/>
-        <v>0.41211637081651037</v>
+        <v>0.3786113309299482</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
@@ -14722,11 +14881,11 @@
       </c>
       <c r="M22" s="8">
         <f t="shared" si="3"/>
-        <v>0.7055595595532197</v>
+        <v>0.64763250181021714</v>
       </c>
       <c r="N22" s="8">
         <f t="shared" si="4"/>
-        <v>1.8011319486419205E-2</v>
+        <v>3.6915210732155979E-2</v>
       </c>
       <c r="O22" s="8"/>
       <c r="T22">
@@ -14734,7 +14893,7 @@
       </c>
       <c r="U22" s="8">
         <f t="shared" si="5"/>
-        <v>0.4750164607107214</v>
+        <v>0.4362971077296689</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
@@ -14779,11 +14938,11 @@
       </c>
       <c r="M23" s="8">
         <f t="shared" si="3"/>
-        <v>1.8322380482922027</v>
+        <v>1.6792083009972278</v>
       </c>
       <c r="N23" s="8">
         <f t="shared" si="4"/>
-        <v>9.5887365811576142E-2</v>
+        <v>2.4532049837752434E-2</v>
       </c>
       <c r="O23" s="8"/>
       <c r="T23">
@@ -14791,7 +14950,7 @@
       </c>
       <c r="U23" s="8">
         <f t="shared" si="5"/>
-        <v>0.57027171395105114</v>
+        <v>0.52363269218996122</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
@@ -14836,11 +14995,11 @@
       </c>
       <c r="M24" s="8">
         <f t="shared" si="3"/>
-        <v>1.4097220493770872</v>
+        <v>1.2925306255770468</v>
       </c>
       <c r="N24" s="8">
         <f t="shared" si="4"/>
-        <v>2.0955690597955758</v>
+        <v>2.4485973860389865</v>
       </c>
       <c r="O24" s="8"/>
       <c r="T24">
@@ -14848,7 +15007,7 @@
       </c>
       <c r="U24" s="8">
         <f t="shared" si="5"/>
-        <v>0.73048092745670445</v>
+        <v>0.67047005065577236</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
@@ -14893,11 +15052,11 @@
       </c>
       <c r="M25" s="8">
         <f t="shared" si="3"/>
-        <v>11.417499278266785</v>
+        <v>10.432893092202438</v>
       </c>
       <c r="N25" s="8">
         <f t="shared" si="4"/>
-        <v>0.57662217430222806</v>
+        <v>5.0737456605688125E-2</v>
       </c>
       <c r="O25" s="8"/>
       <c r="T25">
@@ -14905,7 +15064,7 @@
       </c>
       <c r="U25" s="8">
         <f t="shared" si="5"/>
-        <v>1.049960731199588</v>
+        <v>0.96313678939772329</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
@@ -14950,11 +15109,11 @@
       </c>
       <c r="M26" s="8">
         <f t="shared" si="3"/>
-        <v>13.980902072188034</v>
+        <v>12.771040155814124</v>
       </c>
       <c r="N26" s="8">
         <f t="shared" si="4"/>
-        <v>1.213645271155555</v>
+        <v>1.1708586262532971E-2</v>
       </c>
       <c r="O26" s="8"/>
       <c r="T26">
@@ -14962,7 +15121,7 @@
       </c>
       <c r="U26" s="8">
         <f t="shared" si="5"/>
-        <v>1.3596391829662815</v>
+        <v>1.2466843409678667</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
@@ -15001,25 +15160,21 @@
         <f t="shared" si="1"/>
         <v>16.014354166666696</v>
       </c>
-      <c r="L27" s="2">
-        <f t="shared" si="2"/>
-        <v>263.90172923991076</v>
-      </c>
+      <c r="L27" s="2"/>
       <c r="M27" s="8">
         <f t="shared" si="3"/>
-        <v>5.7295815110622739</v>
-      </c>
-      <c r="N27" s="8">
-        <f t="shared" si="4"/>
-        <v>163.99528342614289</v>
-      </c>
-      <c r="O27" s="8"/>
+        <v>5.2413408612118975</v>
+      </c>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8" t="s">
+        <v>83</v>
+      </c>
       <c r="T27">
         <v>24</v>
       </c>
       <c r="U27" s="8">
         <f t="shared" si="5"/>
-        <v>1.9297003917338651</v>
+        <v>1.7683818531098865</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
@@ -15030,7 +15185,7 @@
       </c>
       <c r="U28" s="8">
         <f t="shared" si="5"/>
-        <v>3.2234376849448614</v>
+        <v>2.9515081702193009</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
@@ -15040,7 +15195,7 @@
       </c>
       <c r="U29" s="8">
         <f t="shared" si="5"/>
-        <v>7.6228912196858145</v>
+        <v>6.9700852166200313</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
@@ -15050,7 +15205,7 @@
       </c>
       <c r="U30" s="8">
         <f t="shared" si="5"/>
-        <v>53.196337169397601</v>
+        <v>48.487681795993666</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
@@ -15060,7 +15215,7 @@
       </c>
       <c r="U31" s="8">
         <f t="shared" si="5"/>
-        <v>116.38904900552225</v>
+        <v>105.95226467469747</v>
       </c>
     </row>
   </sheetData>
@@ -15072,8 +15227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5D3B69-0EAB-9C44-9653-189DB4862E17}">
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AO65" sqref="AO65"/>
+    <sheetView topLeftCell="G46" workbookViewId="0">
+      <selection activeCell="Y77" sqref="Y77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16202,14 +16357,14 @@
         <v>86</v>
       </c>
       <c r="U24">
-        <v>0.64</v>
+        <v>0.26834897977175737</v>
       </c>
       <c r="V24">
-        <v>29.6</v>
+        <v>53.437671059414761</v>
       </c>
       <c r="W24">
         <f>SQRT(V24)</f>
-        <v>5.440588203494177</v>
+        <v>7.310107458814457</v>
       </c>
       <c r="Y24" t="s">
         <v>80</v>
@@ -16278,11 +16433,11 @@
       </c>
       <c r="R25" s="10">
         <f>$U$24*EXP(SQRT($V$24/(25-B25)))</f>
-        <v>1.8999556391241135</v>
+        <v>1.1578380423170569</v>
       </c>
       <c r="S25" s="8">
         <f>(I25-R25)^2</f>
-        <v>0.18713552624008731</v>
+        <v>9.5806318479543018E-2</v>
       </c>
       <c r="T25" s="8"/>
       <c r="U25" t="s">
@@ -16290,14 +16445,14 @@
       </c>
       <c r="V25" s="10">
         <f>(AVERAGE(S25:S51))</f>
-        <v>269.12439715160139</v>
+        <v>145.86315875073683</v>
       </c>
       <c r="Y25">
         <v>0</v>
       </c>
       <c r="Z25" s="8">
         <f>$U$24*EXP(SQRT($V$24/(25-Y25)))</f>
-        <v>1.8999556391241135</v>
+        <v>1.1578380423170569</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
@@ -16362,11 +16517,11 @@
       </c>
       <c r="R26" s="10">
         <f t="shared" ref="R26:R51" si="16">$U$24*EXP(SQRT($V$24/(25-B26)))</f>
-        <v>1.9745541622561826</v>
+        <v>1.2193285053676766</v>
       </c>
       <c r="S26" s="8">
         <f t="shared" ref="S26:S48" si="17">(I26-R26)^2</f>
-        <v>0.37066651972943443</v>
+        <v>2.1433479585689166E-2</v>
       </c>
       <c r="T26" s="8"/>
       <c r="Y26">
@@ -16374,7 +16529,7 @@
       </c>
       <c r="Z26" s="8">
         <f t="shared" ref="Z26:Z51" si="18">$U$24*EXP(SQRT($V$24/(25-Y26)))</f>
-        <v>1.9900384471964747</v>
+        <v>1.2321933481678797</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
@@ -16439,11 +16594,11 @@
       </c>
       <c r="R27" s="10">
         <f t="shared" si="16"/>
-        <v>2.0728255263331379</v>
+        <v>1.30155562877514</v>
       </c>
       <c r="S27" s="8">
         <f t="shared" si="17"/>
-        <v>0.46136097210984256</v>
+        <v>8.4703157476699355E-3</v>
       </c>
       <c r="T27" s="8"/>
       <c r="Y27">
@@ -16451,7 +16606,7 @@
       </c>
       <c r="Z27" s="8">
         <f t="shared" si="18"/>
-        <v>2.0979204176700872</v>
+        <v>1.3227716166041696</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
@@ -16516,11 +16671,11 @@
       </c>
       <c r="R28" s="10">
         <f t="shared" si="16"/>
-        <v>2.1936931541163904</v>
+        <v>1.4045381526406455</v>
       </c>
       <c r="S28" s="8">
         <f t="shared" si="17"/>
-        <v>0.55705697865848736</v>
+        <v>1.8311983400938966E-3</v>
       </c>
       <c r="T28" s="8"/>
       <c r="U28" t="s">
@@ -16535,7 +16690,7 @@
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="18"/>
-        <v>2.2297053189323508</v>
+        <v>1.4356054622129337</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
@@ -16600,11 +16755,11 @@
       </c>
       <c r="R29" s="10">
         <f t="shared" si="16"/>
-        <v>2.3594282773120323</v>
+        <v>1.54893642315251</v>
       </c>
       <c r="S29" s="8">
         <f t="shared" si="17"/>
-        <v>0.98954038026672253</v>
+        <v>3.395343858509467E-2</v>
       </c>
       <c r="T29" s="8"/>
       <c r="U29" t="s">
@@ -16612,14 +16767,14 @@
       </c>
       <c r="V29" s="8">
         <f>SUM(S25:S51)</f>
-        <v>6458.9855316384337</v>
+        <v>3500.7158100176839</v>
       </c>
       <c r="Y29">
         <v>8</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" si="18"/>
-        <v>2.3946793956458774</v>
+        <v>1.5801100545366218</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
@@ -16684,11 +16839,11 @@
       </c>
       <c r="R30" s="10">
         <f t="shared" si="16"/>
-        <v>2.550627300809706</v>
+        <v>1.7198958366777151</v>
       </c>
       <c r="S30" s="8">
         <f t="shared" si="17"/>
-        <v>1.1563586742623919</v>
+        <v>5.9833917841769856E-2</v>
       </c>
       <c r="T30" s="8"/>
       <c r="U30" t="s">
@@ -16696,14 +16851,14 @@
       </c>
       <c r="V30" s="11">
         <f>1-V29/V28</f>
-        <v>0.68421766951478546</v>
+        <v>0.8288486339783766</v>
       </c>
       <c r="Y30">
         <v>10</v>
       </c>
       <c r="Z30" s="8">
         <f t="shared" si="18"/>
-        <v>2.6076951087736537</v>
+        <v>1.7717976409904157</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
@@ -16768,11 +16923,11 @@
       </c>
       <c r="R31" s="10">
         <f t="shared" si="16"/>
-        <v>2.8145408330785351</v>
+        <v>1.9631625761850144</v>
       </c>
       <c r="S31" s="8">
         <f t="shared" si="17"/>
-        <v>1.5988745697275986</v>
+        <v>0.17064158300515239</v>
       </c>
       <c r="T31" s="8"/>
       <c r="Y31">
@@ -16780,7 +16935,7 @@
       </c>
       <c r="Z31" s="8">
         <f t="shared" si="18"/>
-        <v>2.7394885910340814</v>
+        <v>1.893148688695341</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
@@ -16845,11 +17000,11 @@
       </c>
       <c r="R32" s="10">
         <f t="shared" si="16"/>
-        <v>2.97740548046397</v>
+        <v>2.1172960617755763</v>
       </c>
       <c r="S32" s="8">
         <f t="shared" si="17"/>
-        <v>1.899944235445459</v>
+        <v>0.26860921241686259</v>
       </c>
       <c r="T32" s="8"/>
       <c r="U32" t="s">
@@ -16864,7 +17019,7 @@
       </c>
       <c r="Z32" s="8">
         <f t="shared" si="18"/>
-        <v>2.8940606044434345</v>
+        <v>2.0380470862762325</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
@@ -16929,11 +17084,11 @@
       </c>
       <c r="R33" s="10">
         <f t="shared" si="16"/>
-        <v>3.1647259716960243</v>
+        <v>2.298185724365601</v>
       </c>
       <c r="S33" s="8">
         <f t="shared" si="17"/>
-        <v>2.0061964339608016</v>
+        <v>0.30234864907172621</v>
       </c>
       <c r="T33" s="8"/>
       <c r="Y33">
@@ -16941,7 +17096,7 @@
       </c>
       <c r="Z33" s="8">
         <f t="shared" si="18"/>
-        <v>3.0779858223753651</v>
+        <v>2.2139522623931112</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
@@ -17006,11 +17161,11 @@
       </c>
       <c r="R34" s="10">
         <f t="shared" si="16"/>
-        <v>3.4521634068177609</v>
+        <v>2.5829379806927273</v>
       </c>
       <c r="S34" s="8">
         <f t="shared" si="17"/>
-        <v>2.7333129576908051</v>
+        <v>0.61473123602834312</v>
       </c>
       <c r="T34" s="8"/>
       <c r="U34" t="s">
@@ -17021,7 +17176,7 @@
       </c>
       <c r="Z34" s="8">
         <f t="shared" si="18"/>
-        <v>3.3006253875659088</v>
+        <v>2.4317553107640979</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
@@ -17086,11 +17241,11 @@
       </c>
       <c r="R35" s="10">
         <f t="shared" si="16"/>
-        <v>3.7842784272380765</v>
+        <v>2.9222239304157487</v>
       </c>
       <c r="S35" s="8">
         <f t="shared" si="17"/>
-        <v>3.3886697522078819</v>
+        <v>0.95800928215825909</v>
       </c>
       <c r="T35" s="8"/>
       <c r="Y35">
@@ -17098,7 +17253,7 @@
       </c>
       <c r="Z35" s="8">
         <f t="shared" si="18"/>
-        <v>3.5757607502483397</v>
+        <v>2.7079502105487117</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
@@ -17163,11 +17318,11 @@
       </c>
       <c r="R36" s="10">
         <f t="shared" si="16"/>
-        <v>4.172726601942335</v>
+        <v>3.3322124386865966</v>
       </c>
       <c r="S36" s="8">
         <f t="shared" si="17"/>
-        <v>3.9625500323372389</v>
+        <v>1.3227330636908967</v>
       </c>
       <c r="T36" s="8"/>
       <c r="Y36">
@@ -17175,7 +17330,7 @@
       </c>
       <c r="Z36" s="8">
         <f t="shared" si="18"/>
-        <v>3.924513123359898</v>
+        <v>3.0686431832365768</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
@@ -17240,11 +17395,11 @@
       </c>
       <c r="R37" s="10">
         <f t="shared" si="16"/>
-        <v>4.6201800883119022</v>
+        <v>3.820966664073806</v>
       </c>
       <c r="S37" s="8">
         <f t="shared" si="17"/>
-        <v>4.1305243335741197</v>
+        <v>1.5206730268095783</v>
       </c>
       <c r="T37" s="8"/>
       <c r="Y37">
@@ -17252,7 +17407,7 @@
       </c>
       <c r="Z37" s="8">
         <f t="shared" si="18"/>
-        <v>4.3808873865585509</v>
+        <v>3.5574581799120657</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
@@ -17317,11 +17472,11 @@
       </c>
       <c r="R38" s="10">
         <f t="shared" si="16"/>
-        <v>5.3222983896290508</v>
+        <v>4.6208935054069755</v>
       </c>
       <c r="S38" s="8">
         <f t="shared" si="17"/>
-        <v>4.451952538789004</v>
+        <v>1.9840417583521381</v>
       </c>
       <c r="T38" s="8"/>
       <c r="Y38">
@@ -17329,7 +17484,7 @@
       </c>
       <c r="Z38" s="8">
         <f t="shared" si="18"/>
-        <v>5.0031211644183937</v>
+        <v>4.2524442322324365</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
@@ -17394,11 +17549,11 @@
       </c>
       <c r="R39" s="10">
         <f t="shared" si="16"/>
-        <v>5.2493434754496766</v>
+        <v>4.5359887351109913</v>
       </c>
       <c r="S39" s="8">
         <f t="shared" si="17"/>
-        <v>1.8201081689833836</v>
+        <v>0.4041896402024735</v>
       </c>
       <c r="T39" s="8"/>
       <c r="Y39">
@@ -17406,7 +17561,7 @@
       </c>
       <c r="Z39" s="8">
         <f t="shared" si="18"/>
-        <v>5.8992411887604863</v>
+        <v>5.306178471528499</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
@@ -17471,11 +17626,11 @@
       </c>
       <c r="R40" s="10">
         <f t="shared" si="16"/>
-        <v>6.9426124648443945</v>
+        <v>6.6040761733158817</v>
       </c>
       <c r="S40" s="8">
         <f t="shared" si="17"/>
-        <v>2.9835303440570051</v>
+        <v>1.9286365411558368</v>
       </c>
       <c r="T40" s="8"/>
       <c r="Y40">
@@ -17483,7 +17638,7 @@
       </c>
       <c r="Z40" s="8">
         <f t="shared" si="18"/>
-        <v>7.2922920699511531</v>
+        <v>7.0548297833838856</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
@@ -17548,11 +17703,11 @@
       </c>
       <c r="R41" s="10">
         <f t="shared" si="16"/>
-        <v>7.4748044127500046</v>
+        <v>7.2930870054151553</v>
       </c>
       <c r="S41" s="8">
         <f t="shared" si="17"/>
-        <v>1.2270633614967001</v>
+        <v>1.6626718325816661</v>
       </c>
       <c r="T41" s="8"/>
       <c r="Y41">
@@ -17560,7 +17715,7 @@
       </c>
       <c r="Z41" s="8">
         <f t="shared" si="18"/>
-        <v>8.3180742878937561</v>
+        <v>8.4195023344071682</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
@@ -17625,11 +17780,11 @@
       </c>
       <c r="R42" s="10">
         <f t="shared" si="16"/>
-        <v>8.6786677129681813</v>
+        <v>8.9135309724348453</v>
       </c>
       <c r="S42" s="8">
         <f t="shared" si="17"/>
-        <v>0.20742336212280349</v>
+        <v>4.8653017727974285E-2</v>
       </c>
       <c r="T42" s="8"/>
       <c r="Y42">
@@ -17637,7 +17792,7 @@
       </c>
       <c r="Z42" s="8">
         <f t="shared" si="18"/>
-        <v>9.7182639749306965</v>
+        <v>10.376947373809607</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
@@ -17702,11 +17857,11 @@
       </c>
       <c r="R43" s="10">
         <f t="shared" si="16"/>
-        <v>10.523007739772698</v>
+        <v>11.547645680775103</v>
       </c>
       <c r="S43" s="8">
         <f t="shared" si="17"/>
-        <v>8.3980371442834834</v>
+        <v>3.509248257964916</v>
       </c>
       <c r="T43" s="8"/>
       <c r="Y43">
@@ -17714,7 +17869,7 @@
       </c>
       <c r="Z43" s="8">
         <f t="shared" si="18"/>
-        <v>11.726246469384215</v>
+        <v>13.355787529198917</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
@@ -17780,11 +17935,11 @@
       </c>
       <c r="R44" s="10">
         <f t="shared" si="16"/>
-        <v>70.283763785363902</v>
+        <v>148.11562291043342</v>
       </c>
       <c r="S44" s="8">
         <f t="shared" si="17"/>
-        <v>6052.2025051170922</v>
+        <v>1.2928514658137882E-3</v>
       </c>
       <c r="T44" s="8"/>
       <c r="Y44">
@@ -17792,7 +17947,7 @@
       </c>
       <c r="Z44" s="8">
         <f t="shared" si="18"/>
-        <v>14.803119879287109</v>
+        <v>18.265709913727225</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
@@ -17855,11 +18010,11 @@
       </c>
       <c r="R45" s="10">
         <f t="shared" si="16"/>
-        <v>6.6814118192947296</v>
+        <v>6.2724099434435034</v>
       </c>
       <c r="S45" s="8">
         <f t="shared" si="17"/>
-        <v>0.97587097402029277</v>
+        <v>0.33507883412341588</v>
       </c>
       <c r="T45" s="8"/>
       <c r="Y45">
@@ -17867,7 +18022,7 @@
       </c>
       <c r="Z45" s="8">
         <f t="shared" si="18"/>
-        <v>19.978226473463391</v>
+        <v>27.326335837191724</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
@@ -17930,11 +18085,11 @@
       </c>
       <c r="R46" s="10">
         <f t="shared" si="16"/>
-        <v>6.0540433738576942</v>
+        <v>5.4941029054937189</v>
       </c>
       <c r="S46" s="8">
         <f t="shared" si="17"/>
-        <v>0.20091115123164383</v>
+        <v>1.0164099837374043</v>
       </c>
       <c r="T46" s="8"/>
       <c r="Y46">
@@ -17942,7 +18097,7 @@
       </c>
       <c r="Z46" s="8">
         <f t="shared" si="18"/>
-        <v>29.987772333918453</v>
+        <v>47.160636543456711</v>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
@@ -18005,11 +18160,11 @@
       </c>
       <c r="R47" s="10">
         <f t="shared" si="16"/>
-        <v>6.4415874381949259</v>
+        <v>5.9717820132424846</v>
       </c>
       <c r="S47" s="8">
         <f t="shared" si="17"/>
-        <v>2.7452028640484721E-2</v>
+        <v>9.2488297830591704E-2</v>
       </c>
       <c r="T47" s="8"/>
       <c r="Y47">
@@ -18017,7 +18172,7 @@
       </c>
       <c r="Z47" s="8">
         <f t="shared" si="18"/>
-        <v>54.376635317450372</v>
+        <v>104.92132295662176</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
@@ -18080,11 +18235,11 @@
       </c>
       <c r="R48" s="10">
         <f t="shared" si="16"/>
-        <v>47.488259841845128</v>
+        <v>87.462845662527769</v>
       </c>
       <c r="S48" s="8">
         <f t="shared" si="17"/>
-        <v>363.0484860815065</v>
+        <v>3484.3540242807808</v>
       </c>
       <c r="T48" s="8"/>
       <c r="Y48">
@@ -18092,7 +18247,7 @@
       </c>
       <c r="Z48" s="8">
         <f t="shared" si="18"/>
-        <v>147.56977294755592</v>
+        <v>401.27239123622371</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.2">
@@ -18152,7 +18307,7 @@
       <c r="Q49" s="2"/>
       <c r="R49" s="10">
         <f t="shared" si="16"/>
-        <v>88.411542288738772</v>
+        <v>201.60363749963926</v>
       </c>
       <c r="S49" s="8"/>
       <c r="T49" s="8" t="s">
@@ -18163,7 +18318,7 @@
       </c>
       <c r="Z49" s="8">
         <f t="shared" si="18"/>
-        <v>342.39430962585197</v>
+        <v>1243.2920704084856</v>
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.2">
@@ -18223,7 +18378,7 @@
       <c r="Q50" s="2"/>
       <c r="R50" s="10">
         <f t="shared" si="16"/>
-        <v>275.80085538115776</v>
+        <v>929.74803249015952</v>
       </c>
       <c r="S50" s="8"/>
       <c r="T50" s="8"/>
@@ -18232,7 +18387,7 @@
       </c>
       <c r="Z50" s="8">
         <f t="shared" si="18"/>
-        <v>1405.1038899233204</v>
+        <v>8288.1836967509298</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.2">
@@ -18292,7 +18447,7 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="10">
         <f t="shared" si="16"/>
-        <v>6534.661079842148</v>
+        <v>65365.46627206893</v>
       </c>
       <c r="S51" s="8"/>
       <c r="T51" s="8"/>
@@ -18301,7 +18456,7 @@
       </c>
       <c r="Z51" s="8">
         <f t="shared" si="18"/>
-        <v>13184.834077730731</v>
+        <v>167862.78930883235</v>
       </c>
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.2">
@@ -18466,21 +18621,21 @@
       </c>
       <c r="R55" s="8">
         <f>$U$55*EXP(SQRT($V$55/(25-B55)))</f>
-        <v>0.85659488186816957</v>
+        <v>0.85796747744169655</v>
       </c>
       <c r="S55" s="8">
         <f>(R55-F55)^2</f>
-        <v>2.8825712190406225E-4</v>
-      </c>
-      <c r="U55">
+        <v>3.3674937075955913E-4</v>
+      </c>
+      <c r="U55" s="2">
         <v>0.2</v>
       </c>
       <c r="V55">
-        <v>52.9</v>
+        <v>53.016516163804141</v>
       </c>
       <c r="W55">
         <f>SQRT(V55)</f>
-        <v>7.2732386183872721</v>
+        <v>7.2812441357095112</v>
       </c>
       <c r="X55" s="8"/>
       <c r="Z55">
@@ -18488,7 +18643,7 @@
       </c>
       <c r="AA55" s="8">
         <f>$U$55*EXP(SQRT($V$55/(25-Z55)))</f>
-        <v>0.85659488186816957</v>
+        <v>0.85796747744169655</v>
       </c>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.2">
@@ -18555,25 +18710,25 @@
       </c>
       <c r="R56" s="8">
         <f t="shared" ref="R56:R78" si="29">$U$55*EXP(SQRT($V$55/(25-B56)))</f>
-        <v>0.88087083338532135</v>
+        <v>0.88230946741795457</v>
       </c>
       <c r="S56" s="8">
         <f t="shared" ref="S56:S78" si="30">(R56-F56)^2</f>
-        <v>2.0547868302995956E-4</v>
+        <v>2.4879262955599789E-4</v>
       </c>
       <c r="U56" t="s">
         <v>74</v>
       </c>
       <c r="V56">
         <f>SQRT(AVERAGE(S55:S78))</f>
-        <v>0.44782693207265267</v>
+        <v>0.44750341746402633</v>
       </c>
       <c r="Z56">
         <v>2</v>
       </c>
       <c r="AA56" s="8">
         <f t="shared" ref="AA56:AA76" si="31">$U$55*EXP(SQRT($V$55/(25-Z56)))</f>
-        <v>0.9113185030920562</v>
+        <v>0.91284100623760323</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.2">
@@ -18640,18 +18795,18 @@
       </c>
       <c r="R57" s="8">
         <f t="shared" si="29"/>
-        <v>0.90698511618533473</v>
+        <v>0.90849561345916641</v>
       </c>
       <c r="S57" s="8">
         <f t="shared" si="30"/>
-        <v>1.134775282391407E-4</v>
+        <v>1.4794052593492787E-4</v>
       </c>
       <c r="Z57">
         <v>4</v>
       </c>
       <c r="AA57" s="8">
         <f t="shared" si="31"/>
-        <v>0.97795939721747871</v>
+        <v>0.97966933370008658</v>
       </c>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.2">
@@ -18718,25 +18873,25 @@
       </c>
       <c r="R58" s="8">
         <f t="shared" si="29"/>
-        <v>0.93450540637837598</v>
+        <v>0.93609253382740365</v>
       </c>
       <c r="S58" s="8">
         <f t="shared" si="30"/>
-        <v>7.3376569104794848E-5</v>
+        <v>1.030862495854936E-4</v>
       </c>
       <c r="U58" t="s">
         <v>67</v>
       </c>
       <c r="V58" s="8">
         <f>SUM(S55:S80)</f>
-        <v>4.8131750661505031</v>
+        <v>4.8062234074075834</v>
       </c>
       <c r="Z58">
         <v>6</v>
       </c>
       <c r="AA58" s="8">
         <f t="shared" si="31"/>
-        <v>1.0609422865512206</v>
+        <v>1.0628925946877905</v>
       </c>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.2">
@@ -18803,18 +18958,18 @@
       </c>
       <c r="R59" s="8">
         <f t="shared" si="29"/>
-        <v>0.95791671028641279</v>
+        <v>0.95956973173904903</v>
       </c>
       <c r="S59" s="8">
         <f t="shared" si="30"/>
-        <v>1.6966796570278316E-5</v>
+        <v>3.3317122282235322E-5</v>
       </c>
       <c r="Z59">
         <v>8</v>
       </c>
       <c r="AA59" s="8">
         <f t="shared" si="31"/>
-        <v>1.1671694707523836</v>
+        <v>1.1694378754947772</v>
       </c>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.2">
@@ -18881,11 +19036,11 @@
       </c>
       <c r="R60" s="8">
         <f t="shared" si="29"/>
-        <v>1.0087368423804699</v>
+        <v>1.0105350568751041</v>
       </c>
       <c r="S60" s="8">
         <f t="shared" si="30"/>
-        <v>9.0656960540867952E-7</v>
+        <v>7.1584291614044825E-7</v>
       </c>
       <c r="U60" t="s">
         <v>68</v>
@@ -18899,7 +19054,7 @@
       </c>
       <c r="AA60" s="8">
         <f t="shared" si="31"/>
-        <v>1.3080065016455373</v>
+        <v>1.3107129677901646</v>
       </c>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.2">
@@ -18966,25 +19121,25 @@
       </c>
       <c r="R61" s="8">
         <f t="shared" si="29"/>
-        <v>1.052313918733554</v>
+        <v>1.0542388898176827</v>
       </c>
       <c r="S61" s="8">
         <f t="shared" si="30"/>
-        <v>1.367392310637386E-4</v>
+        <v>9.5425233831354794E-5</v>
       </c>
       <c r="U61" t="s">
         <v>69</v>
       </c>
       <c r="V61">
         <f>1-V58/V60</f>
-        <v>0.97915319757942687</v>
+        <v>0.9791833065728287</v>
       </c>
       <c r="Z61">
         <v>11</v>
       </c>
       <c r="AA61" s="8">
         <f t="shared" si="31"/>
-        <v>1.3971254466858716</v>
+        <v>1.400117886813798</v>
       </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.2">
@@ -19051,18 +19206,18 @@
       </c>
       <c r="R62" s="8">
         <f t="shared" si="29"/>
-        <v>1.0943655238037189</v>
+        <v>1.0964147043195629</v>
       </c>
       <c r="S62" s="8">
         <f t="shared" si="30"/>
-        <v>2.1252723761867184E-4</v>
+        <v>1.5697918460564893E-4</v>
       </c>
       <c r="Z62">
         <v>12</v>
       </c>
       <c r="AA62" s="8">
         <f t="shared" si="31"/>
-        <v>1.5034997121182974</v>
+        <v>1.5068416879331217</v>
       </c>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.2">
@@ -19129,11 +19284,11 @@
       </c>
       <c r="R63" s="8">
         <f t="shared" si="29"/>
-        <v>1.1432245328704091</v>
+        <v>1.1454202664806405</v>
       </c>
       <c r="S63" s="8">
         <f t="shared" si="30"/>
-        <v>6.2952376398771369E-4</v>
+        <v>5.241617266991197E-4</v>
       </c>
       <c r="U63" t="s">
         <v>66</v>
@@ -19143,7 +19298,7 @@
       </c>
       <c r="AA63" s="8">
         <f t="shared" si="31"/>
-        <v>1.6325859411442676</v>
+        <v>1.6363632000465422</v>
       </c>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.2">
@@ -19210,11 +19365,11 @@
       </c>
       <c r="R64" s="8">
         <f t="shared" si="29"/>
-        <v>1.2040284953492915</v>
+        <v>1.2064098207320277</v>
       </c>
       <c r="S64" s="8">
         <f t="shared" si="30"/>
-        <v>1.0572313634701384E-3</v>
+        <v>9.0804403484218469E-4</v>
       </c>
       <c r="U64" s="2">
         <f>AVERAGE(F55:F78)</f>
@@ -19225,7 +19380,7 @@
       </c>
       <c r="AA64" s="8">
         <f t="shared" si="31"/>
-        <v>1.7923471947038476</v>
+        <v>1.7966787059364735</v>
       </c>
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.2">
@@ -19292,18 +19447,18 @@
       </c>
       <c r="R65" s="8">
         <f t="shared" si="29"/>
-        <v>1.1111506595667044</v>
+        <v>1.1132499210220268</v>
       </c>
       <c r="S65" s="8">
         <f t="shared" si="30"/>
-        <v>5.6496882532591232E-4</v>
+        <v>4.6958072695422787E-4</v>
       </c>
       <c r="Z65">
         <v>15</v>
       </c>
       <c r="AA65" s="8">
         <f t="shared" si="31"/>
-        <v>1.9948364909629437</v>
+        <v>1.9998929505941458</v>
       </c>
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.2">
@@ -19370,18 +19525,18 @@
       </c>
       <c r="R66" s="8">
         <f t="shared" si="29"/>
-        <v>1.3878894911328894</v>
+        <v>1.3908519953514793</v>
       </c>
       <c r="S66" s="8">
         <f t="shared" si="30"/>
-        <v>1.9692900220654808E-4</v>
+        <v>1.2255896394050897E-4</v>
       </c>
       <c r="Z66">
         <v>16</v>
       </c>
       <c r="AA66" s="8">
         <f t="shared" si="31"/>
-        <v>2.2591191041161394</v>
+        <v>2.2651556271559667</v>
       </c>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.2">
@@ -19448,18 +19603,18 @@
       </c>
       <c r="R67" s="8">
         <f t="shared" si="29"/>
-        <v>1.5150062370948216</v>
+        <v>1.5183865312571967</v>
       </c>
       <c r="S67" s="8">
         <f t="shared" si="30"/>
-        <v>8.3081573803497587E-3</v>
+        <v>8.9358052712887638E-3</v>
       </c>
       <c r="Z67">
         <v>17</v>
       </c>
       <c r="AA67" s="8">
         <f t="shared" si="31"/>
-        <v>2.6170304571965448</v>
+        <v>2.624448134548178</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.2">
@@ -19526,11 +19681,11 @@
       </c>
       <c r="R68" s="8">
         <f t="shared" si="29"/>
-        <v>1.7108794062031423</v>
+        <v>1.7149262266662366</v>
       </c>
       <c r="S68" s="8">
         <f t="shared" si="30"/>
-        <v>9.7645638914529848E-3</v>
+        <v>8.9811609803182348E-3</v>
       </c>
       <c r="U68" t="s">
         <v>76</v>
@@ -19540,7 +19695,7 @@
       </c>
       <c r="AA68" s="8">
         <f t="shared" si="31"/>
-        <v>3.1254800551394446</v>
+        <v>3.1349514583053786</v>
       </c>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.2">
@@ -19607,18 +19762,18 @@
       </c>
       <c r="R69" s="8">
         <f t="shared" si="29"/>
-        <v>1.8116085194839315</v>
+        <v>1.8160079447003754</v>
       </c>
       <c r="S69" s="8">
         <f t="shared" si="30"/>
-        <v>1.0377904383302885E-2</v>
+        <v>9.500902834268932E-3</v>
       </c>
       <c r="Z69">
         <v>19</v>
       </c>
       <c r="AA69" s="8">
         <f t="shared" si="31"/>
-        <v>3.8956062662854523</v>
+        <v>3.9083588656012545</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.2">
@@ -19685,18 +19840,18 @@
       </c>
       <c r="R70" s="8">
         <f t="shared" si="29"/>
-        <v>7.4234133668053808</v>
+        <v>7.4530021212838058</v>
       </c>
       <c r="S70" s="8">
         <f t="shared" si="30"/>
-        <v>0.43816489261841246</v>
+        <v>0.47821236199603268</v>
       </c>
       <c r="Z70">
         <v>20</v>
       </c>
       <c r="AA70" s="8">
         <f t="shared" si="31"/>
-        <v>5.1719680377304753</v>
+        <v>5.1905177803911755</v>
       </c>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.2">
@@ -19763,18 +19918,18 @@
       </c>
       <c r="R71" s="8">
         <f t="shared" si="29"/>
-        <v>1.6037718359236941</v>
+        <v>1.6074509225788365</v>
       </c>
       <c r="S71" s="8">
         <f t="shared" si="30"/>
-        <v>2.7585551674143625E-3</v>
+        <v>2.3856252398465941E-3</v>
       </c>
       <c r="Z71">
         <v>21</v>
       </c>
       <c r="AA71" s="8">
         <f t="shared" si="31"/>
-        <v>7.5926554870463709</v>
+        <v>7.6231079608503665</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.2">
@@ -19841,18 +19996,18 @@
       </c>
       <c r="R72" s="8">
         <f t="shared" si="29"/>
-        <v>2.214315273272498</v>
+        <v>2.220183124994032</v>
       </c>
       <c r="S72" s="8">
         <f t="shared" si="30"/>
-        <v>1.3201007603452302E-3</v>
+        <v>9.2813689073020528E-4</v>
       </c>
       <c r="Z72">
         <v>22</v>
       </c>
       <c r="AA72" s="8">
         <f t="shared" si="31"/>
-        <v>13.326684276109573</v>
+        <v>13.388422612332803</v>
       </c>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.2">
@@ -19919,18 +20074,18 @@
       </c>
       <c r="R73" s="8">
         <f t="shared" si="29"/>
-        <v>2.5589861107748111</v>
+        <v>2.5661759151791914</v>
       </c>
       <c r="S73" s="8">
         <f t="shared" si="30"/>
-        <v>2.8065828698186734E-3</v>
+        <v>2.0964848607691578E-3</v>
       </c>
       <c r="Z73">
         <v>22.5</v>
       </c>
       <c r="AA73" s="8">
         <f t="shared" si="31"/>
-        <v>19.896863128386755</v>
+        <v>19.997859069180794</v>
       </c>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.2">
@@ -19997,18 +20152,18 @@
       </c>
       <c r="R74" s="8">
         <f t="shared" si="29"/>
-        <v>3.0932561878353879</v>
+        <v>3.102594548866211</v>
       </c>
       <c r="S74" s="8">
         <f t="shared" si="30"/>
-        <v>6.2509009565315408E-3</v>
+        <v>7.8147368857095362E-3</v>
       </c>
       <c r="Z74">
         <v>23</v>
       </c>
       <c r="AA74" s="8">
         <f t="shared" si="31"/>
-        <v>34.244242069471774</v>
+        <v>34.438640054667047</v>
       </c>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.2">
@@ -20075,18 +20230,18 @@
       </c>
       <c r="R75" s="8">
         <f t="shared" si="29"/>
-        <v>3.7497548665822364</v>
+        <v>3.7618720042102876</v>
       </c>
       <c r="S75" s="8">
         <f t="shared" si="30"/>
-        <v>5.2932706113990192E-3</v>
+        <v>7.2032570986710611E-3</v>
       </c>
       <c r="Z75">
         <v>23.5</v>
       </c>
       <c r="AA75" s="8">
         <f t="shared" si="31"/>
-        <v>75.878740909612404</v>
+        <v>76.376345111619628</v>
       </c>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.2">
@@ -20153,18 +20308,18 @@
       </c>
       <c r="R76" s="8">
         <f t="shared" si="29"/>
-        <v>11.424594041223768</v>
+        <v>11.475575261002524</v>
       </c>
       <c r="S76" s="8">
         <f t="shared" si="30"/>
-        <v>1.4114594443084685</v>
+        <v>1.5351948612891775</v>
       </c>
       <c r="Z76">
         <v>24</v>
       </c>
       <c r="AA76" s="8">
         <f t="shared" si="31"/>
-        <v>288.2420867248768</v>
+        <v>290.55887491390115</v>
       </c>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.2">
@@ -20231,11 +20386,11 @@
       </c>
       <c r="R77" s="8">
         <f t="shared" si="29"/>
-        <v>11.769933854961559</v>
+        <v>11.822843647376388</v>
       </c>
       <c r="S77" s="8">
         <f t="shared" si="30"/>
-        <v>2.8861785382035348</v>
+        <v>2.7092036663822201</v>
       </c>
       <c r="AA77" s="8"/>
     </row>
@@ -20303,11 +20458,11 @@
       </c>
       <c r="R78" s="8">
         <f t="shared" si="29"/>
-        <v>4.6876423638273179</v>
+        <v>4.7039459255775835</v>
       </c>
       <c r="S78" s="8">
         <f t="shared" si="30"/>
-        <v>2.6995772307346649E-2</v>
+        <v>3.2619056066643379E-2</v>
       </c>
       <c r="AA78" s="8"/>
     </row>
@@ -20370,8 +20525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8740C2-F49F-1743-9D8F-C5BD1AAB3FF1}">
   <dimension ref="A1:Y82"/>
   <sheetViews>
-    <sheetView topLeftCell="K50" workbookViewId="0">
-      <selection activeCell="AL69" sqref="AL69"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="P72" sqref="P72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21647,14 +21802,14 @@
         <v>81</v>
       </c>
       <c r="T27">
-        <v>4.4999999999999998E-2</v>
+        <v>8.6217039355890576E-2</v>
       </c>
       <c r="U27">
-        <v>23</v>
+        <v>17.419398569252852</v>
       </c>
       <c r="V27" s="2">
         <f>SQRT(U27)</f>
-        <v>4.7958315233127191</v>
+        <v>4.1736553007229586</v>
       </c>
       <c r="X27" t="s">
         <v>80</v>
@@ -21723,11 +21878,11 @@
       </c>
       <c r="R28" s="8">
         <f>$T$27*EXP(SQRT($U$27/(25-B28)))</f>
-        <v>0.11742840097313823</v>
+        <v>0.19866080851497578</v>
       </c>
       <c r="S28" s="8">
         <f>(I28-R28)^2</f>
-        <v>2.0520185142472486E-3</v>
+        <v>1.2911946160744348E-3</v>
       </c>
       <c r="T28" s="8"/>
       <c r="U28" t="s">
@@ -21735,14 +21890,14 @@
       </c>
       <c r="V28" s="10">
         <f>SQRT(AVERAGE($S$28:$S$54))</f>
-        <v>0.37830464410647446</v>
+        <v>0.3253704556671933</v>
       </c>
       <c r="X28">
         <v>0</v>
       </c>
       <c r="Y28" s="8">
         <f>$T$27*EXP(SQRT($U$27/(25-X28)))</f>
-        <v>0.11742840097313823</v>
+        <v>0.19866080851497578</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
@@ -21807,11 +21962,11 @@
       </c>
       <c r="R29" s="8">
         <f t="shared" ref="R29:R54" si="15">$T$27*EXP(SQRT($U$27/(25-B29)))</f>
-        <v>0.12109383522426401</v>
+        <v>0.2040465698445314</v>
       </c>
       <c r="S29" s="8">
         <f t="shared" ref="S29:S53" si="16">(I29-R29)^2</f>
-        <v>1.7569262936744795E-3</v>
+        <v>1.6840378313570114E-3</v>
       </c>
       <c r="T29" s="8"/>
       <c r="X29">
@@ -21819,7 +21974,7 @@
       </c>
       <c r="Y29" s="8">
         <f t="shared" ref="Y29:Y54" si="17">$T$27*EXP(SQRT($U$27/(25-X29)))</f>
-        <v>0.12232268228065703</v>
+        <v>0.20584740049479477</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
@@ -21884,11 +22039,11 @@
       </c>
       <c r="R30" s="8">
         <f t="shared" si="15"/>
-        <v>0.12573642680883065</v>
+        <v>0.21083789201321357</v>
       </c>
       <c r="S30" s="8">
         <f t="shared" si="16"/>
-        <v>2.2430665090876706E-3</v>
+        <v>1.4243409702271569E-3</v>
       </c>
       <c r="T30" s="8"/>
       <c r="U30" t="s">
@@ -21903,7 +22058,7 @@
       </c>
       <c r="Y30" s="8">
         <f t="shared" si="17"/>
-        <v>0.12814965065137718</v>
+        <v>0.214355121253333</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
@@ -21968,11 +22123,11 @@
       </c>
       <c r="R31" s="8">
         <f t="shared" si="15"/>
-        <v>0.13162271630348066</v>
+        <v>0.21940203206943787</v>
       </c>
       <c r="S31" s="8">
         <f t="shared" si="16"/>
-        <v>1.1781291253087874E-3</v>
+        <v>2.8574830101364391E-3</v>
       </c>
       <c r="T31" s="8"/>
       <c r="U31" t="s">
@@ -21980,14 +22135,14 @@
       </c>
       <c r="V31" s="8">
         <f>SUM(S28:S54)</f>
-        <v>3.7209744975656838</v>
+        <v>2.7525142689480018</v>
       </c>
       <c r="X31">
         <v>6</v>
       </c>
       <c r="Y31" s="8">
         <f t="shared" si="17"/>
-        <v>0.13521981292977017</v>
+        <v>0.22461100160663416</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
@@ -22052,11 +22207,11 @@
       </c>
       <c r="R32" s="8">
         <f t="shared" si="15"/>
-        <v>0.13923083693480162</v>
+        <v>0.23039824007541498</v>
       </c>
       <c r="S32" s="8">
         <f t="shared" si="16"/>
-        <v>9.7634991680839792E-4</v>
+        <v>3.5905028307188632E-3</v>
       </c>
       <c r="T32" s="8"/>
       <c r="U32" t="s">
@@ -22064,14 +22219,14 @@
       </c>
       <c r="V32" s="10">
         <f>1-$V$31/$V$30</f>
-        <v>0.96019707812350219</v>
+        <v>0.97055660809216582</v>
       </c>
       <c r="X32">
         <v>8</v>
       </c>
       <c r="Y32" s="8">
         <f t="shared" si="17"/>
-        <v>0.14400132282894418</v>
+        <v>0.23725320053219492</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
@@ -22136,11 +22291,11 @@
       </c>
       <c r="R33" s="8">
         <f t="shared" si="15"/>
-        <v>0.1479572611692633</v>
+        <v>0.24291534678755292</v>
       </c>
       <c r="S33" s="8">
         <f t="shared" si="16"/>
-        <v>9.6572831297133646E-4</v>
+        <v>4.0808992024657246E-3</v>
       </c>
       <c r="T33" s="8"/>
       <c r="X33">
@@ -22148,7 +22303,7 @@
       </c>
       <c r="Y33" s="8">
         <f t="shared" si="17"/>
-        <v>0.14924964453554718</v>
+        <v>0.24476086083799128</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
@@ -22213,11 +22368,11 @@
       </c>
       <c r="R34" s="8">
         <f t="shared" si="15"/>
-        <v>0.16052901738333822</v>
+        <v>0.26078189659547185</v>
       </c>
       <c r="S34" s="8">
         <f t="shared" si="16"/>
-        <v>3.5602245014466037E-4</v>
+        <v>6.6234078722430022E-3</v>
       </c>
       <c r="T34" s="8"/>
       <c r="U34" t="s">
@@ -22232,7 +22387,7 @@
       </c>
       <c r="Y34" s="8">
         <f t="shared" si="17"/>
-        <v>0.15523511902118128</v>
+        <v>0.25328136750761765</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
@@ -22297,11 +22452,11 @@
       </c>
       <c r="R35" s="8">
         <f t="shared" si="15"/>
-        <v>0.16657180908324268</v>
+        <v>0.2693044005017417</v>
       </c>
       <c r="S35" s="8">
         <f t="shared" si="16"/>
-        <v>1.4440756304539374E-4</v>
+        <v>8.2293240066023763E-3</v>
       </c>
       <c r="T35" s="8"/>
       <c r="X35">
@@ -22309,7 +22464,7 @@
       </c>
       <c r="Y35" s="8">
         <f t="shared" si="17"/>
-        <v>0.16213063168105551</v>
+        <v>0.2630447393908687</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
@@ -22374,11 +22529,11 @@
       </c>
       <c r="R36" s="8">
         <f t="shared" si="15"/>
-        <v>0.17555804066831784</v>
+        <v>0.2819046717201551</v>
       </c>
       <c r="S36" s="8">
         <f t="shared" si="16"/>
-        <v>3.1258826248512654E-5</v>
+        <v>1.0151705383779863E-2</v>
       </c>
       <c r="T36" s="8"/>
       <c r="U36" t="s">
@@ -22389,7 +22544,7 @@
       </c>
       <c r="Y36" s="8">
         <f t="shared" si="17"/>
-        <v>0.17016811042738117</v>
+        <v>0.27435737301277496</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
@@ -22454,11 +22609,11 @@
       </c>
       <c r="R37" s="8">
         <f t="shared" si="15"/>
-        <v>0.18483956705795485</v>
+        <v>0.29483145967434815</v>
       </c>
       <c r="S37" s="8">
         <f t="shared" si="16"/>
-        <v>4.7920965204676637E-5</v>
+        <v>1.3668974507643835E-2</v>
       </c>
       <c r="T37" s="8"/>
       <c r="X37">
@@ -22466,7 +22621,7 @@
       </c>
       <c r="Y37" s="8">
         <f t="shared" si="17"/>
-        <v>0.1796660410712573</v>
+        <v>0.28763673183316124</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.2">
@@ -22531,11 +22686,11 @@
       </c>
       <c r="R38" s="8">
         <f t="shared" si="15"/>
-        <v>0.20075713126648911</v>
+        <v>0.31680758099235085</v>
       </c>
       <c r="S38" s="8">
         <f t="shared" si="16"/>
-        <v>1.3253020775826744E-4</v>
+        <v>1.6272223609540459E-2</v>
       </c>
       <c r="T38" s="8"/>
       <c r="X38">
@@ -22543,7 +22698,7 @@
       </c>
       <c r="Y38" s="8">
         <f t="shared" si="17"/>
-        <v>0.19107386876364749</v>
+        <v>0.30346681151082383</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.2">
@@ -22608,11 +22763,11 @@
       </c>
       <c r="R39" s="8">
         <f t="shared" si="15"/>
-        <v>0.21647360910649308</v>
+        <v>0.33828510404413403</v>
       </c>
       <c r="S39" s="8">
         <f t="shared" si="16"/>
-        <v>4.8631193327804389E-4</v>
+        <v>2.0696843670589753E-2</v>
       </c>
       <c r="T39" s="8"/>
       <c r="W39" s="10"/>
@@ -22621,7 +22776,7 @@
       </c>
       <c r="Y39" s="8">
         <f t="shared" si="17"/>
-        <v>0.20504666319571263</v>
+        <v>0.32269045573721539</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.2">
@@ -22686,11 +22841,11 @@
       </c>
       <c r="R40" s="8">
         <f t="shared" si="15"/>
-        <v>0.2570125188384208</v>
+        <v>0.39279025929361461</v>
       </c>
       <c r="S40" s="8">
         <f t="shared" si="16"/>
-        <v>1.5926705263504995E-3</v>
+        <v>3.0865576523425475E-2</v>
       </c>
       <c r="T40" s="8"/>
       <c r="X40">
@@ -22698,7 +22853,7 @@
       </c>
       <c r="Y40" s="8">
         <f t="shared" si="17"/>
-        <v>0.22257697515745176</v>
+        <v>0.34657050100986875</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
@@ -22763,11 +22918,11 @@
       </c>
       <c r="R41" s="8">
         <f t="shared" si="15"/>
-        <v>0.29114771444373133</v>
+        <v>0.43781799599176424</v>
       </c>
       <c r="S41" s="8">
         <f t="shared" si="16"/>
-        <v>2.0051088864440235E-3</v>
+        <v>3.6652613827252975E-2</v>
       </c>
       <c r="T41" s="8"/>
       <c r="X41">
@@ -22775,7 +22930,7 @@
       </c>
       <c r="Y41" s="8">
         <f t="shared" si="17"/>
-        <v>0.24524187919723919</v>
+        <v>0.3770877101157093</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.2">
@@ -22840,11 +22995,11 @@
       </c>
       <c r="R42" s="8">
         <f t="shared" si="15"/>
-        <v>0.28762691574815696</v>
+        <v>0.43320677248306472</v>
       </c>
       <c r="S42" s="8">
         <f t="shared" si="16"/>
-        <v>8.8947982115307469E-5</v>
+        <v>1.8536450253658705E-2</v>
       </c>
       <c r="T42" s="8"/>
       <c r="X42">
@@ -22852,7 +23007,7 @@
       </c>
       <c r="Y42" s="8">
         <f t="shared" si="17"/>
-        <v>0.27570085635048086</v>
+        <v>0.41753202867476052</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.2">
@@ -22917,11 +23072,11 @@
       </c>
       <c r="R43" s="8">
         <f t="shared" si="15"/>
-        <v>0.36800895268502243</v>
+        <v>0.53683268895952896</v>
       </c>
       <c r="S43" s="8">
         <f t="shared" si="16"/>
-        <v>3.4702837815519654E-4</v>
+        <v>2.2558549611129981E-2</v>
       </c>
       <c r="T43" s="8"/>
       <c r="X43">
@@ -22929,7 +23084,7 @@
       </c>
       <c r="Y43" s="8">
         <f t="shared" si="17"/>
-        <v>0.31879635409633084</v>
+        <v>0.47378587161692465</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
@@ -22994,11 +23149,11 @@
       </c>
       <c r="R44" s="8">
         <f t="shared" si="15"/>
-        <v>0.3927660154367914</v>
+        <v>0.56812802408998786</v>
       </c>
       <c r="S44" s="8">
         <f t="shared" si="16"/>
-        <v>4.5088533099351021E-2</v>
+        <v>1.3674166866233706E-3</v>
       </c>
       <c r="T44" s="8"/>
       <c r="X44">
@@ -23006,7 +23161,7 @@
       </c>
       <c r="Y44" s="8">
         <f t="shared" si="17"/>
-        <v>0.38430001965780758</v>
+        <v>0.55745580346230017</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.2">
@@ -23071,11 +23226,11 @@
       </c>
       <c r="R45" s="8">
         <f t="shared" si="15"/>
-        <v>0.44802418931343574</v>
+        <v>0.63708483824133189</v>
       </c>
       <c r="S45" s="8">
         <f t="shared" si="16"/>
-        <v>1.5683424362184447E-2</v>
+        <v>4.0739075701699918E-3</v>
       </c>
       <c r="T45" s="8"/>
       <c r="X45">
@@ -23083,7 +23238,7 @@
       </c>
       <c r="Y45" s="8">
         <f t="shared" si="17"/>
-        <v>0.49501014208860411</v>
+        <v>0.69484964278191119</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
@@ -23148,11 +23303,11 @@
       </c>
       <c r="R46" s="8">
         <f t="shared" si="15"/>
-        <v>0.53097085107353326</v>
+        <v>0.73857772669513744</v>
       </c>
       <c r="S46" s="8">
         <f t="shared" si="16"/>
-        <v>6.3747897138584564E-3</v>
+        <v>1.6323791833127828E-2</v>
       </c>
       <c r="T46" s="8"/>
       <c r="X46">
@@ -23160,7 +23315,7 @@
       </c>
       <c r="Y46" s="8">
         <f t="shared" si="17"/>
-        <v>0.58414092731773515</v>
+        <v>0.80253898113566569</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.2">
@@ -23225,11 +23380,11 @@
       </c>
       <c r="R47" s="8">
         <f t="shared" si="15"/>
-        <v>2.8317175846553231</v>
+        <v>3.1700234476264111</v>
       </c>
       <c r="S47" s="8">
         <f t="shared" si="16"/>
-        <v>2.8985908294110692</v>
+        <v>1.8610934161592301</v>
       </c>
       <c r="T47" s="8"/>
       <c r="X47">
@@ -23237,7 +23392,7 @@
       </c>
       <c r="Y47" s="8">
         <f t="shared" si="17"/>
-        <v>0.71733080698263818</v>
+        <v>0.95961181360154468</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
@@ -23302,11 +23457,11 @@
       </c>
       <c r="R48" s="8">
         <f t="shared" si="15"/>
-        <v>0.35577663653791253</v>
+        <v>0.52126983617331546</v>
       </c>
       <c r="S48" s="8">
         <f t="shared" si="16"/>
-        <v>2.2336090172636624E-3</v>
+        <v>1.3978835778355589E-2</v>
       </c>
       <c r="T48" s="8"/>
       <c r="X48">
@@ -23314,7 +23469,7 @@
       </c>
       <c r="Y48" s="8">
         <f t="shared" si="17"/>
-        <v>0.93431409083768935</v>
+        <v>1.2077558102414399</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
@@ -23379,11 +23534,11 @@
       </c>
       <c r="R49" s="8">
         <f t="shared" si="15"/>
-        <v>0.32615915507444265</v>
+        <v>0.48329452382557198</v>
       </c>
       <c r="S49" s="8">
         <f t="shared" si="16"/>
-        <v>1.6070030555310165E-2</v>
+        <v>9.2219990672764215E-4</v>
       </c>
       <c r="T49" s="8"/>
       <c r="X49">
@@ -23391,7 +23546,7 @@
       </c>
       <c r="Y49" s="8">
         <f t="shared" si="17"/>
-        <v>1.3365239847154058</v>
+        <v>1.6492695896613865</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.2">
@@ -23456,11 +23611,11 @@
       </c>
       <c r="R50" s="8">
         <f t="shared" si="15"/>
-        <v>0.34449542170583353</v>
+        <v>0.50685542591005428</v>
       </c>
       <c r="S50" s="8">
         <f t="shared" si="16"/>
-        <v>8.7477449010118537E-3</v>
+        <v>4.7376548446599947E-3</v>
       </c>
       <c r="T50" s="8"/>
       <c r="X50">
@@ -23468,7 +23623,7 @@
       </c>
       <c r="Y50" s="8">
         <f t="shared" si="17"/>
-        <v>2.2584692307802929</v>
+        <v>2.6035810765574894</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
@@ -23533,11 +23688,11 @@
       </c>
       <c r="R51" s="8">
         <f t="shared" si="15"/>
-        <v>2.0042851121817606</v>
+        <v>2.3466249105750436</v>
       </c>
       <c r="S51" s="8">
         <f t="shared" si="16"/>
-        <v>0.2369186497490412</v>
+        <v>2.0852255471395135E-2</v>
       </c>
       <c r="T51" s="8"/>
       <c r="X51">
@@ -23545,7 +23700,7 @@
       </c>
       <c r="Y51" s="8">
         <f t="shared" si="17"/>
-        <v>5.4452231282351118</v>
+        <v>5.6000070250749356</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
@@ -23610,11 +23765,11 @@
       </c>
       <c r="R52" s="8">
         <f t="shared" si="15"/>
-        <v>3.4665226295426446</v>
+        <v>3.7801612249455663</v>
       </c>
       <c r="S52" s="8">
         <f t="shared" si="16"/>
-        <v>0.22440228369717427</v>
+        <v>0.6199196715531583</v>
       </c>
       <c r="T52" s="8"/>
       <c r="X52">
@@ -23622,7 +23777,7 @@
       </c>
       <c r="Y52" s="8">
         <f t="shared" si="17"/>
-        <v>11.434744147696952</v>
+        <v>10.680659411215686</v>
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
@@ -23687,11 +23842,11 @@
       </c>
       <c r="R53" s="8">
         <f t="shared" si="15"/>
-        <v>9.4498985982421537</v>
+        <v>9.0477489379514981</v>
       </c>
       <c r="S53" s="8">
         <f t="shared" si="16"/>
-        <v>0.25246017666857712</v>
+        <v>1.0060991417707586E-2</v>
       </c>
       <c r="T53" s="8"/>
       <c r="X53">
@@ -23699,7 +23854,7 @@
       </c>
       <c r="Y53" s="8">
         <f t="shared" si="17"/>
-        <v>39.695474704878798</v>
+        <v>31.549334095708467</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
@@ -23761,7 +23916,7 @@
       <c r="Q54" s="2"/>
       <c r="R54" s="8">
         <f t="shared" si="15"/>
-        <v>153.86838091968809</v>
+        <v>102.58001698462988</v>
       </c>
       <c r="S54" s="8"/>
       <c r="T54" s="8" t="s">
@@ -23772,7 +23927,7 @@
       </c>
       <c r="Y54" s="8">
         <f t="shared" si="17"/>
-        <v>285.67579059652263</v>
+        <v>175.76181179179352</v>
       </c>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
@@ -23924,28 +24079,28 @@
       </c>
       <c r="Q58" s="8">
         <f t="shared" ref="Q58:Q67" si="28">$T$58*EXP($U$58/(25-B58)^2)</f>
-        <v>0.14717334522585371</v>
+        <v>0.14621813470219469</v>
       </c>
       <c r="R58" s="8">
         <f>(Q58-F58)^2</f>
-        <v>5.0150549661396726E-5</v>
+        <v>6.4592015622185506E-5</v>
       </c>
       <c r="T58">
-        <v>0.14099999999999999</v>
+        <v>0.14008677250699564</v>
       </c>
       <c r="U58">
-        <v>22.8</v>
+        <v>22.792723825980826</v>
       </c>
       <c r="V58">
         <f>SQRT(U58)</f>
-        <v>4.7749345545253288</v>
+        <v>4.7741725802468462</v>
       </c>
       <c r="X58">
         <v>0</v>
       </c>
       <c r="Y58" s="8">
         <f>$T$58*EXP($U$58/(25-X58)^2)</f>
-        <v>0.14623865206421349</v>
+        <v>0.14528980346200421</v>
       </c>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
@@ -24008,25 +24163,25 @@
       </c>
       <c r="Q59" s="8">
         <f t="shared" si="28"/>
-        <v>0.14864062195049707</v>
+        <v>0.14767542072330003</v>
       </c>
       <c r="R59" s="8">
         <f t="shared" ref="R59:R67" si="29">(Q59-F59)^2</f>
-        <v>5.0740130791590542E-5</v>
+        <v>6.5422407634601419E-5</v>
       </c>
       <c r="T59" t="s">
         <v>74</v>
       </c>
       <c r="U59" s="9">
         <f>SQRT(AVERAGE(R59:R76))</f>
-        <v>7.6866573643982533E-3</v>
+        <v>7.590371378968527E-3</v>
       </c>
       <c r="X59">
         <v>2</v>
       </c>
       <c r="Y59" s="8">
         <f t="shared" ref="Y59:Y82" si="30">$T$58*EXP($U$58/(25-X59)^2)</f>
-        <v>0.14720999126222756</v>
+        <v>0.14625453127156215</v>
       </c>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
@@ -24089,18 +24244,18 @@
       </c>
       <c r="Q60" s="8">
         <f t="shared" si="28"/>
-        <v>0.1501780100350841</v>
+        <v>0.14920233579094061</v>
       </c>
       <c r="R60" s="8">
         <f t="shared" si="29"/>
-        <v>3.2384398491318224E-5</v>
+        <v>4.4440934485995633E-5</v>
       </c>
       <c r="X60">
         <v>4</v>
       </c>
       <c r="Y60" s="8">
         <f t="shared" si="30"/>
-        <v>0.14848152959128577</v>
+        <v>0.14751741184844255</v>
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
@@ -24163,25 +24318,25 @@
       </c>
       <c r="Q61" s="8">
         <f t="shared" si="28"/>
-        <v>0.15283121090954824</v>
+        <v>0.15183745078836772</v>
       </c>
       <c r="R61" s="8">
         <f t="shared" si="29"/>
-        <v>2.4156272286666051E-5</v>
+        <v>3.4912300826033823E-5</v>
       </c>
       <c r="T61" t="s">
         <v>67</v>
       </c>
       <c r="U61" s="8">
         <f>SUM(R58:R67)</f>
-        <v>5.8191286260031775E-4</v>
+        <v>5.831156546581667E-4</v>
       </c>
       <c r="X61">
         <v>6</v>
       </c>
       <c r="Y61" s="8">
         <f t="shared" si="30"/>
-        <v>0.15019249706430657</v>
+        <v>0.14921672410761161</v>
       </c>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
@@ -24244,18 +24399,18 @@
       </c>
       <c r="Q62" s="8">
         <f t="shared" si="28"/>
-        <v>0.1557794589761802</v>
+        <v>0.15476558463723794</v>
       </c>
       <c r="R62" s="8">
         <f t="shared" si="29"/>
-        <v>8.4633190138150983E-7</v>
+        <v>3.7397268114719493E-6</v>
       </c>
       <c r="X62">
         <v>8</v>
       </c>
       <c r="Y62" s="8">
         <f t="shared" si="30"/>
-        <v>0.15257444241745477</v>
+        <v>0.15158243323310053</v>
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
@@ -24318,11 +24473,11 @@
       </c>
       <c r="Q63" s="8">
         <f t="shared" si="28"/>
-        <v>0.16107768299180808</v>
+        <v>0.16002761765655721</v>
       </c>
       <c r="R63" s="8">
         <f t="shared" si="29"/>
-        <v>8.6005743010992173E-6</v>
+        <v>3.5442137866796975E-6</v>
       </c>
       <c r="T63" t="s">
         <v>68</v>
@@ -24336,7 +24491,7 @@
       </c>
       <c r="Y63" s="8">
         <f t="shared" si="30"/>
-        <v>0.15603701015760224</v>
+        <v>0.15502137784877004</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
@@ -24399,25 +24554,25 @@
       </c>
       <c r="Q64" s="8">
         <f t="shared" si="28"/>
-        <v>0.16742357574146213</v>
+        <v>0.1663300904599726</v>
       </c>
       <c r="R64" s="8">
         <f t="shared" si="29"/>
-        <v>6.0527757687800303E-5</v>
+        <v>4.4708927046395202E-5</v>
       </c>
       <c r="T64" t="s">
         <v>69</v>
       </c>
       <c r="U64">
         <f>1-U61/U63</f>
-        <v>0.96175907166043462</v>
+        <v>0.96168002909607875</v>
       </c>
       <c r="X64">
         <v>12</v>
       </c>
       <c r="Y64" s="8">
         <f t="shared" si="30"/>
-        <v>0.16136536358835915</v>
+        <v>0.16031333157292713</v>
       </c>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
@@ -24480,18 +24635,18 @@
       </c>
       <c r="Q65" s="8">
         <f t="shared" si="28"/>
-        <v>0.18412872798368593</v>
+        <v>0.18292058509943579</v>
       </c>
       <c r="R65" s="8">
         <f t="shared" si="29"/>
-        <v>1.4589808063760601E-4</v>
+        <v>1.1817179019151766E-4</v>
       </c>
       <c r="X65">
         <v>14</v>
       </c>
       <c r="Y65" s="8">
         <f t="shared" si="30"/>
-        <v>0.17023666950675909</v>
+        <v>0.16912391187647993</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
@@ -24554,11 +24709,11 @@
       </c>
       <c r="Q66" s="8">
         <f t="shared" si="28"/>
-        <v>0.22282872394589739</v>
+        <v>0.22135317838641089</v>
       </c>
       <c r="R66" s="8">
         <f t="shared" si="29"/>
-        <v>1.5737903355018867E-4</v>
+        <v>1.2253459391544733E-4</v>
       </c>
       <c r="T66" t="s">
         <v>66</v>
@@ -24568,7 +24723,7 @@
       </c>
       <c r="Y66" s="8">
         <f t="shared" si="30"/>
-        <v>0.1771080308859605</v>
+        <v>0.17594813647485316</v>
       </c>
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.2">
@@ -24631,11 +24786,11 @@
       </c>
       <c r="Q67" s="8">
         <f t="shared" si="28"/>
-        <v>0.2758358384299977</v>
+        <v>0.27399062572185084</v>
       </c>
       <c r="R67" s="8">
         <f t="shared" si="29"/>
-        <v>5.122973329127054E-5</v>
+        <v>8.1048744337838477E-5</v>
       </c>
       <c r="T67" s="2">
         <f>AVERAGE(F58:F67)</f>
@@ -24646,7 +24801,7 @@
       </c>
       <c r="Y67" s="8">
         <f t="shared" si="30"/>
-        <v>0.18683789548827009</v>
+        <v>0.18561111147189799</v>
       </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.2">
@@ -24657,7 +24812,7 @@
       </c>
       <c r="Y68" s="8">
         <f t="shared" si="30"/>
-        <v>0.20134299376219839</v>
+        <v>0.2000161961486889</v>
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
@@ -24671,7 +24826,7 @@
       </c>
       <c r="Y69" s="8">
         <f t="shared" si="30"/>
-        <v>0.22454272768279698</v>
+        <v>0.22305528674002914</v>
       </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.2">
@@ -24682,7 +24837,7 @@
       </c>
       <c r="Y70" s="8">
         <f t="shared" si="30"/>
-        <v>0.24187108093313855</v>
+        <v>0.24026315156303191</v>
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.2">
@@ -24693,7 +24848,7 @@
       </c>
       <c r="Y71" s="8">
         <f t="shared" si="30"/>
-        <v>0.26562704107905971</v>
+        <v>0.26385329597369095</v>
       </c>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.2">
@@ -24704,7 +24859,7 @@
       </c>
       <c r="Y72" s="8">
         <f t="shared" si="30"/>
-        <v>0.29960918198176956</v>
+        <v>0.29759708498030712</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
@@ -24715,7 +24870,7 @@
       </c>
       <c r="Y73" s="8">
         <f t="shared" si="30"/>
-        <v>0.35099075720791428</v>
+        <v>0.34861598513540876</v>
       </c>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
@@ -24726,7 +24881,7 @@
       </c>
       <c r="Y74" s="8">
         <f t="shared" si="30"/>
-        <v>0.43471290135251767</v>
+        <v>0.431742196575855</v>
       </c>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
@@ -24737,7 +24892,7 @@
       </c>
       <c r="Y75" s="8">
         <f t="shared" si="30"/>
-        <v>0.58625795582859697</v>
+        <v>0.58219606553133818</v>
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
@@ -24748,7 +24903,7 @@
       </c>
       <c r="Y76" s="8">
         <f t="shared" si="30"/>
-        <v>0.90685664189406989</v>
+        <v>0.90044812010764819</v>
       </c>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
@@ -24758,7 +24913,7 @@
       </c>
       <c r="Y77" s="8">
         <f t="shared" si="30"/>
-        <v>1.2208953622494321</v>
+        <v>1.2121525770273505</v>
       </c>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
@@ -24768,7 +24923,7 @@
       </c>
       <c r="Y78" s="8">
         <f t="shared" si="30"/>
-        <v>1.7759543576695722</v>
+        <v>1.7630259539968887</v>
       </c>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
@@ -24778,7 +24933,7 @@
       </c>
       <c r="Y79" s="8">
         <f t="shared" si="30"/>
-        <v>2.8745054568774306</v>
+        <v>2.8531414477224541</v>
       </c>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
@@ -24788,7 +24943,7 @@
       </c>
       <c r="Y80" s="8">
         <f t="shared" si="30"/>
-        <v>5.4140888997139065</v>
+        <v>5.3727644295247794</v>
       </c>
     </row>
     <row r="81" spans="17:25" x14ac:dyDescent="0.2">
@@ -24798,7 +24953,7 @@
       </c>
       <c r="Y81" s="8">
         <f t="shared" si="30"/>
-        <v>12.739511620896922</v>
+        <v>12.638822023231807</v>
       </c>
     </row>
     <row r="82" spans="17:25" x14ac:dyDescent="0.2">
@@ -24808,7 +24963,7 @@
       </c>
       <c r="Y82" s="8">
         <f t="shared" si="30"/>
-        <v>42.140303536355496</v>
+        <v>41.791280268171271</v>
       </c>
     </row>
   </sheetData>
@@ -24821,10 +24976,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93670F2-E445-AB45-8D21-2093323B1235}">
-  <dimension ref="A2:F27"/>
+  <dimension ref="A2:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24832,51 +24987,95 @@
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>49</v>
       </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
       </c>
+      <c r="H3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>65</v>
       </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>87</v>
       </c>
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
         <v>84</v>
       </c>
+      <c r="I6" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
+      <c r="I9" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -24895,13 +25094,19 @@
       <c r="F10" t="s">
         <v>11</v>
       </c>
+      <c r="I10" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>52</v>
       </c>
+      <c r="I11" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>18</v>
       </c>
@@ -24921,7 +25126,7 @@
         <v>5.0021092506336498</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>19</v>
       </c>
@@ -24941,7 +25146,7 @@
         <v>5.03519755307026</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>20</v>
       </c>
@@ -24961,7 +25166,7 @@
         <v>5.40073056683016</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>21</v>
       </c>
@@ -24981,7 +25186,7 @@
         <v>5.4848060522174604</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>22</v>
       </c>

</xml_diff>